<commit_message>
completed journal scraping work
</commit_message>
<xml_diff>
--- a/journal_URL.xlsx
+++ b/journal_URL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="122">
   <si>
     <t>journal</t>
   </si>
@@ -222,7 +222,169 @@
     <t>poultry science</t>
   </si>
   <si>
-    <t>Animal feed science and technology</t>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117301669</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116308197</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117304583</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117304315</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117301827</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116303248</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117303115</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116310860</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117301463</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117305497</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117304935</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117304972</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117305540</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117305990</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117305448</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117304364</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117307629</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117307459</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116309245</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116308264</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116306630</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116308628</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116305715</t>
+  </si>
+  <si>
+    <t>animal feed science and technology</t>
+  </si>
+  <si>
+    <t>livestock science</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302858</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302676</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302688</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302597</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302937</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302998</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302949</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302986</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317303104</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302913</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317303050</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302925</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317303256</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317303268</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317303220</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317303049</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317303098</t>
+  </si>
+  <si>
+    <t>revista brasileira de zootecnia</t>
+  </si>
+  <si>
+    <t>http://www.scielo.br/scielo.php?script=sci_arttext&amp;pid=S1516-35982017000900731&amp;lng=en&amp;nrm=iso&amp;tlng=en</t>
+  </si>
+  <si>
+    <t>http://www.scielo.br/scielo.php?script=sci_arttext&amp;pid=S1516-35982017000900740&amp;lng=en&amp;nrm=iso&amp;tlng=en</t>
+  </si>
+  <si>
+    <t>http://www.scielo.br/scielo.php?script=sci_arttext&amp;pid=S1516-35982017000900755&amp;lng=en&amp;nrm=iso&amp;tlng=en</t>
+  </si>
+  <si>
+    <t>http://www.scielo.br/scielo.php?script=sci_arttext&amp;pid=S1516-35982017000900760&amp;lng=en&amp;nrm=iso&amp;tlng=en</t>
+  </si>
+  <si>
+    <t>http://www.scielo.br/scielo.php?script=sci_arttext&amp;pid=S1516-35982017000900766&amp;lng=en&amp;nrm=iso&amp;tlng=en</t>
+  </si>
+  <si>
+    <t>journal of animal science and biotechnology</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1186/s40104-017-0213-1</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1186/s40104-017-0212-2</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1186/s40104-017-0205-1</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1186/s40104-017-0204-2</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1186/s40104-017-0200-6</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1186/s40104-017-0198-9</t>
   </si>
 </sst>
 </file>
@@ -551,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,13 +1728,1022 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51">
+        <v>2017</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B51">
-        <v>2017</v>
-      </c>
-      <c r="C51">
-        <v>10</v>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52">
+        <v>2017</v>
+      </c>
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53">
+        <v>2017</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54">
+        <v>2017</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55">
+        <v>2017</v>
+      </c>
+      <c r="C55">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56">
+        <v>2017</v>
+      </c>
+      <c r="C56">
+        <v>10</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" t="s">
+        <v>40</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57">
+        <v>2017</v>
+      </c>
+      <c r="C57">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" t="s">
+        <v>40</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58">
+        <v>2017</v>
+      </c>
+      <c r="C58">
+        <v>10</v>
+      </c>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59">
+        <v>2017</v>
+      </c>
+      <c r="C59">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60">
+        <v>2017</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>90</v>
+      </c>
+      <c r="B61">
+        <v>2017</v>
+      </c>
+      <c r="C61">
+        <v>10</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62">
+        <v>2017</v>
+      </c>
+      <c r="C62">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>90</v>
+      </c>
+      <c r="B63">
+        <v>2017</v>
+      </c>
+      <c r="C63">
+        <v>10</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>40</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>90</v>
+      </c>
+      <c r="B64">
+        <v>2017</v>
+      </c>
+      <c r="C64">
+        <v>10</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65">
+        <v>2017</v>
+      </c>
+      <c r="C65">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" t="s">
+        <v>40</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>90</v>
+      </c>
+      <c r="B66">
+        <v>2017</v>
+      </c>
+      <c r="C66">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>90</v>
+      </c>
+      <c r="B67">
+        <v>2017</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>40</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>90</v>
+      </c>
+      <c r="B68">
+        <v>2017</v>
+      </c>
+      <c r="C68">
+        <v>10</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>40</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69">
+        <v>2017</v>
+      </c>
+      <c r="C69">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>90</v>
+      </c>
+      <c r="B70">
+        <v>2017</v>
+      </c>
+      <c r="C70">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>90</v>
+      </c>
+      <c r="B71">
+        <v>2017</v>
+      </c>
+      <c r="C71">
+        <v>10</v>
+      </c>
+      <c r="D71" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" t="s">
+        <v>40</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>90</v>
+      </c>
+      <c r="B72">
+        <v>2017</v>
+      </c>
+      <c r="C72">
+        <v>10</v>
+      </c>
+      <c r="D72" t="s">
+        <v>15</v>
+      </c>
+      <c r="E72" t="s">
+        <v>40</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>90</v>
+      </c>
+      <c r="B73">
+        <v>2017</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E73" t="s">
+        <v>40</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74">
+        <v>2017</v>
+      </c>
+      <c r="C74">
+        <v>11</v>
+      </c>
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" t="s">
+        <v>21</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75">
+        <v>2017</v>
+      </c>
+      <c r="C75">
+        <v>11</v>
+      </c>
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" t="s">
+        <v>40</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76">
+        <v>2017</v>
+      </c>
+      <c r="C76">
+        <v>11</v>
+      </c>
+      <c r="D76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" t="s">
+        <v>40</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>91</v>
+      </c>
+      <c r="B77">
+        <v>2017</v>
+      </c>
+      <c r="C77">
+        <v>11</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" t="s">
+        <v>40</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>91</v>
+      </c>
+      <c r="B78">
+        <v>2017</v>
+      </c>
+      <c r="C78">
+        <v>12</v>
+      </c>
+      <c r="D78" t="s">
+        <v>15</v>
+      </c>
+      <c r="E78" t="s">
+        <v>40</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79">
+        <v>2017</v>
+      </c>
+      <c r="C79">
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>15</v>
+      </c>
+      <c r="E79" t="s">
+        <v>40</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B80">
+        <v>2017</v>
+      </c>
+      <c r="C80">
+        <v>12</v>
+      </c>
+      <c r="D80" t="s">
+        <v>15</v>
+      </c>
+      <c r="E80" t="s">
+        <v>40</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81">
+        <v>2017</v>
+      </c>
+      <c r="C81">
+        <v>12</v>
+      </c>
+      <c r="D81" t="s">
+        <v>15</v>
+      </c>
+      <c r="E81" t="s">
+        <v>40</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>91</v>
+      </c>
+      <c r="B82">
+        <v>2017</v>
+      </c>
+      <c r="C82">
+        <v>12</v>
+      </c>
+      <c r="D82" t="s">
+        <v>15</v>
+      </c>
+      <c r="E82" t="s">
+        <v>40</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83">
+        <v>2017</v>
+      </c>
+      <c r="C83">
+        <v>12</v>
+      </c>
+      <c r="D83" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" t="s">
+        <v>40</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B84">
+        <v>2017</v>
+      </c>
+      <c r="C84">
+        <v>12</v>
+      </c>
+      <c r="D84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" t="s">
+        <v>40</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85">
+        <v>2017</v>
+      </c>
+      <c r="C85">
+        <v>12</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" t="s">
+        <v>40</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86">
+        <v>2017</v>
+      </c>
+      <c r="C86">
+        <v>12</v>
+      </c>
+      <c r="D86" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" t="s">
+        <v>40</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87">
+        <v>2017</v>
+      </c>
+      <c r="C87">
+        <v>12</v>
+      </c>
+      <c r="D87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" t="s">
+        <v>40</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88">
+        <v>2017</v>
+      </c>
+      <c r="C88">
+        <v>12</v>
+      </c>
+      <c r="D88" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" t="s">
+        <v>40</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>91</v>
+      </c>
+      <c r="B89">
+        <v>2017</v>
+      </c>
+      <c r="C89">
+        <v>12</v>
+      </c>
+      <c r="D89" t="s">
+        <v>15</v>
+      </c>
+      <c r="E89" t="s">
+        <v>40</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90">
+        <v>2017</v>
+      </c>
+      <c r="C90">
+        <v>12</v>
+      </c>
+      <c r="D90" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" t="s">
+        <v>40</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>109</v>
+      </c>
+      <c r="B91">
+        <v>2017</v>
+      </c>
+      <c r="C91">
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" t="s">
+        <v>40</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>109</v>
+      </c>
+      <c r="B92">
+        <v>2017</v>
+      </c>
+      <c r="C92">
+        <v>9</v>
+      </c>
+      <c r="D92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" t="s">
+        <v>40</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>109</v>
+      </c>
+      <c r="B93">
+        <v>2017</v>
+      </c>
+      <c r="C93">
+        <v>9</v>
+      </c>
+      <c r="D93" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" t="s">
+        <v>40</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>109</v>
+      </c>
+      <c r="B94">
+        <v>2017</v>
+      </c>
+      <c r="C94">
+        <v>9</v>
+      </c>
+      <c r="D94" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" t="s">
+        <v>40</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>109</v>
+      </c>
+      <c r="B95">
+        <v>2017</v>
+      </c>
+      <c r="C95">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>15</v>
+      </c>
+      <c r="E95" t="s">
+        <v>40</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>115</v>
+      </c>
+      <c r="B96">
+        <v>2017</v>
+      </c>
+      <c r="C96">
+        <v>12</v>
+      </c>
+      <c r="D96" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" t="s">
+        <v>40</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>115</v>
+      </c>
+      <c r="B97">
+        <v>2017</v>
+      </c>
+      <c r="C97">
+        <v>12</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" t="s">
+        <v>40</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>115</v>
+      </c>
+      <c r="B98">
+        <v>2017</v>
+      </c>
+      <c r="C98">
+        <v>12</v>
+      </c>
+      <c r="D98" t="s">
+        <v>15</v>
+      </c>
+      <c r="E98" t="s">
+        <v>21</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>115</v>
+      </c>
+      <c r="B99">
+        <v>2017</v>
+      </c>
+      <c r="C99">
+        <v>12</v>
+      </c>
+      <c r="D99" t="s">
+        <v>15</v>
+      </c>
+      <c r="E99" t="s">
+        <v>40</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>115</v>
+      </c>
+      <c r="B100">
+        <v>2017</v>
+      </c>
+      <c r="C100">
+        <v>12</v>
+      </c>
+      <c r="D100" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100" t="s">
+        <v>40</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>115</v>
+      </c>
+      <c r="B101">
+        <v>2017</v>
+      </c>
+      <c r="C101">
+        <v>12</v>
+      </c>
+      <c r="D101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" t="s">
+        <v>40</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1626,6 +2797,56 @@
     <hyperlink ref="F48" r:id="rId47" xr:uid="{0911262C-9291-4D25-8FD3-4DD54927E0A9}"/>
     <hyperlink ref="F49" r:id="rId48" xr:uid="{6764B081-9680-401A-B2E4-05CBE3478A28}"/>
     <hyperlink ref="F50" r:id="rId49" xr:uid="{79757497-6319-40CF-91FC-5B0FCE9A4FE2}"/>
+    <hyperlink ref="F51" r:id="rId50" xr:uid="{E9EC211A-778D-4FF4-A0FF-D68C546C60D7}"/>
+    <hyperlink ref="F52" r:id="rId51" xr:uid="{E3F1F429-77D4-433A-A867-B20AC7336703}"/>
+    <hyperlink ref="F54" r:id="rId52" xr:uid="{A56E4B61-66B3-4801-9B83-704EC1478358}"/>
+    <hyperlink ref="F55" r:id="rId53" xr:uid="{86B0FAD7-91C0-408D-8D6C-52025AEDCFDA}"/>
+    <hyperlink ref="F56" r:id="rId54" xr:uid="{447483DA-DA6D-471D-8845-33FF43EDA4FD}"/>
+    <hyperlink ref="F57" r:id="rId55" xr:uid="{258D0DAD-5C9E-4B64-83A6-FB9D99645189}"/>
+    <hyperlink ref="F58" r:id="rId56" xr:uid="{996A4E21-1618-455C-A53A-03400E13AF23}"/>
+    <hyperlink ref="F59" r:id="rId57" xr:uid="{391F6D79-404C-461A-BB20-4EBB8C6FB343}"/>
+    <hyperlink ref="F60" r:id="rId58" xr:uid="{CE2318F5-F76D-4E79-BE49-4C20111A8203}"/>
+    <hyperlink ref="F61" r:id="rId59" xr:uid="{C708E0CF-D8F9-4731-98B1-DC882AE35C54}"/>
+    <hyperlink ref="F62" r:id="rId60" xr:uid="{530BCAE5-C742-464A-8127-9E2EC25A1C13}"/>
+    <hyperlink ref="F63" r:id="rId61" xr:uid="{8EBBE48A-894E-415C-B936-B6A1030FD43F}"/>
+    <hyperlink ref="F64" r:id="rId62" xr:uid="{8891EBBA-B3DC-4D1E-B5EB-3FD15172A97B}"/>
+    <hyperlink ref="F66" r:id="rId63" xr:uid="{0975F3B9-16C0-48A2-A8BF-692C0E4775DC}"/>
+    <hyperlink ref="F68" r:id="rId64" xr:uid="{32D58151-4BE3-444C-B904-C41D7DA6D6F7}"/>
+    <hyperlink ref="F69" r:id="rId65" xr:uid="{7431CF82-9DAD-4C1D-8E64-39D57EA5BD7F}"/>
+    <hyperlink ref="F70" r:id="rId66" xr:uid="{6439771A-2E8A-40FE-82B4-52AC1D6BA790}"/>
+    <hyperlink ref="F71" r:id="rId67" xr:uid="{745697D9-69D1-4E16-BC70-F7ED572BBEFA}"/>
+    <hyperlink ref="F67" r:id="rId68" xr:uid="{BE201561-4731-4415-A358-B3BB1C54D00D}"/>
+    <hyperlink ref="F65" r:id="rId69" xr:uid="{B05D08F4-F20A-470E-B406-3EA52B2B0080}"/>
+    <hyperlink ref="F72" r:id="rId70" xr:uid="{85ABB6E7-3274-4D05-BD1B-CF61C65D8368}"/>
+    <hyperlink ref="F73" r:id="rId71" xr:uid="{456B7448-3982-41E8-B6AF-1A27A2799148}"/>
+    <hyperlink ref="F74" r:id="rId72" xr:uid="{130BC4E6-1E9D-46AE-8B67-A90D11AAE02B}"/>
+    <hyperlink ref="F75" r:id="rId73" xr:uid="{48396521-C3F1-4F23-89EE-6461F69D223F}"/>
+    <hyperlink ref="F76" r:id="rId74" xr:uid="{9475EFFC-8BA1-416A-A37E-D75B24B032C0}"/>
+    <hyperlink ref="F77" r:id="rId75" xr:uid="{05486821-1F77-481F-A114-E5EE70CA1B25}"/>
+    <hyperlink ref="F78" r:id="rId76" xr:uid="{EBA50494-1EEB-40B0-A191-7F68A58F5451}"/>
+    <hyperlink ref="F79" r:id="rId77" xr:uid="{204AD702-73DA-47C4-834F-5FB159E6F12B}"/>
+    <hyperlink ref="F80" r:id="rId78" xr:uid="{658F3699-221F-460E-910A-C6F9BD37260A}"/>
+    <hyperlink ref="F81" r:id="rId79" xr:uid="{8DDA15FC-A05F-4432-8055-9FD29BA07E3C}"/>
+    <hyperlink ref="F82" r:id="rId80" xr:uid="{628CD18D-A198-4EB8-A756-92DB0C19B008}"/>
+    <hyperlink ref="F83" r:id="rId81" xr:uid="{3F52D683-167F-48AF-BA6D-F91D0DABB80A}"/>
+    <hyperlink ref="F84" r:id="rId82" xr:uid="{FB7552A3-5CBE-4B66-B900-B2C389633001}"/>
+    <hyperlink ref="F85" r:id="rId83" xr:uid="{14A1314D-20C7-48F6-8B72-8F701A4E9C06}"/>
+    <hyperlink ref="F86" r:id="rId84" xr:uid="{DA6ADD3D-7B2E-4A7D-9249-9E53157EE858}"/>
+    <hyperlink ref="F87" r:id="rId85" xr:uid="{AC2BE3A9-349D-4804-BACF-45C992004529}"/>
+    <hyperlink ref="F88" r:id="rId86" xr:uid="{1AF6A21B-2A05-4068-B566-F3EB51C153EB}"/>
+    <hyperlink ref="F89" r:id="rId87" xr:uid="{3FBE427C-9ED7-4F1D-A571-3A163F493FEF}"/>
+    <hyperlink ref="F90" r:id="rId88" xr:uid="{E2971E7E-9D62-4903-9692-AC35D68F7A8A}"/>
+    <hyperlink ref="F91" r:id="rId89" xr:uid="{9B28AF9D-5E7B-432A-BC18-BB0072878C53}"/>
+    <hyperlink ref="F92" r:id="rId90" xr:uid="{09B3EA5D-37CF-4782-AE71-E6A5CE294321}"/>
+    <hyperlink ref="F93" r:id="rId91" xr:uid="{09062D93-99A2-4962-8AC4-E7FA48C46F82}"/>
+    <hyperlink ref="F94" r:id="rId92" xr:uid="{64687159-E647-4A7E-9E2C-D20F4184EC7D}"/>
+    <hyperlink ref="F95" r:id="rId93" xr:uid="{2DB0AE86-04B9-4F24-B1EC-6D6904FC15B8}"/>
+    <hyperlink ref="F96" r:id="rId94" xr:uid="{660A3532-65A6-469E-B0E6-6FCAF860448E}"/>
+    <hyperlink ref="F97" r:id="rId95" xr:uid="{54A85090-C406-43B6-8B01-D9F8964C7491}"/>
+    <hyperlink ref="F98" r:id="rId96" xr:uid="{C956CFDB-07C0-44B7-9AA0-5DC556AA2BBE}"/>
+    <hyperlink ref="F99" r:id="rId97" xr:uid="{88BD12A1-9F16-437A-8628-00E913A3824F}"/>
+    <hyperlink ref="F100" r:id="rId98" xr:uid="{D2612746-B977-4D18-89A2-9B318417785B}"/>
+    <hyperlink ref="F101" r:id="rId99" xr:uid="{906F1653-D166-4689-9E77-BA736B9A224A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add Dec 2017 reports(w/o JAS et al.)
</commit_message>
<xml_diff>
--- a/journal_URL.xlsx
+++ b/journal_URL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="175">
   <si>
     <t>journal</t>
   </si>
@@ -385,6 +385,165 @@
   </si>
   <si>
     <t>https://link.springer.com/article/10.1186/s40104-017-0198-9</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/237B657E2F9A04A32E300DDE92DAF471</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/05C62A1D1900FC479D7FA09EF35FE30C</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/6488CC1E7DDA4524B4B823176456E44D</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/4E9F1F44E21B84DB41F4B455627FE911</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/E7B351A993E4CC7953EB645EA0A1C04D</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/AE50AAE4EE28F2BC731B039E33C16360</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/0CAD203DE104AD7D49B997863D7437CB</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/CCD30741185B903FBE2577182CA20501</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/09EE760DC9DC60824667D16128E84C71</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/F7444DCBF8954FFA0ED466D1FB38E2D7</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/758770BB19B65FB59AAF4E35E9CC1922</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117305941</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S037784011630952X</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117303322</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117302250</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117302638</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S037784011630219X</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117303437</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117304133</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117310556</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117307915</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117305382</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117305072</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117303346</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117310647</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117306867</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117306880</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117305898</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S037784011730723X</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117309380</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308131</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117310192</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117302614</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117307484</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117307149</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308532</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S037784011630534X</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308039</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117300834</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116311452</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117306624</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23826</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23783</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23761</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23784</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23754</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309037</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217308949</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217308950</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217308809</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217308925</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309219</t>
   </si>
 </sst>
 </file>
@@ -713,10 +872,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E159" sqref="E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2744,6 +2904,1046 @@
       </c>
       <c r="F101" s="1" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>57</v>
+      </c>
+      <c r="B102">
+        <v>2017</v>
+      </c>
+      <c r="C102">
+        <v>12</v>
+      </c>
+      <c r="D102" t="s">
+        <v>162</v>
+      </c>
+      <c r="E102" t="s">
+        <v>21</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>57</v>
+      </c>
+      <c r="B103">
+        <v>2017</v>
+      </c>
+      <c r="C103">
+        <v>12</v>
+      </c>
+      <c r="D103" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103" t="s">
+        <v>40</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>57</v>
+      </c>
+      <c r="B104">
+        <v>2017</v>
+      </c>
+      <c r="C104">
+        <v>12</v>
+      </c>
+      <c r="D104" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" t="s">
+        <v>40</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>57</v>
+      </c>
+      <c r="B105">
+        <v>2017</v>
+      </c>
+      <c r="C105">
+        <v>12</v>
+      </c>
+      <c r="D105" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" t="s">
+        <v>40</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>57</v>
+      </c>
+      <c r="B106">
+        <v>2017</v>
+      </c>
+      <c r="C106">
+        <v>12</v>
+      </c>
+      <c r="D106" t="s">
+        <v>15</v>
+      </c>
+      <c r="E106" t="s">
+        <v>40</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>57</v>
+      </c>
+      <c r="B107">
+        <v>2017</v>
+      </c>
+      <c r="C107">
+        <v>12</v>
+      </c>
+      <c r="D107" t="s">
+        <v>15</v>
+      </c>
+      <c r="E107" t="s">
+        <v>40</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>57</v>
+      </c>
+      <c r="B108">
+        <v>2017</v>
+      </c>
+      <c r="C108">
+        <v>12</v>
+      </c>
+      <c r="D108" t="s">
+        <v>15</v>
+      </c>
+      <c r="E108" t="s">
+        <v>40</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>57</v>
+      </c>
+      <c r="B109">
+        <v>2017</v>
+      </c>
+      <c r="C109">
+        <v>12</v>
+      </c>
+      <c r="D109" t="s">
+        <v>15</v>
+      </c>
+      <c r="E109" t="s">
+        <v>40</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>57</v>
+      </c>
+      <c r="B110">
+        <v>2017</v>
+      </c>
+      <c r="C110">
+        <v>12</v>
+      </c>
+      <c r="D110" t="s">
+        <v>15</v>
+      </c>
+      <c r="E110" t="s">
+        <v>40</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>57</v>
+      </c>
+      <c r="B111">
+        <v>2017</v>
+      </c>
+      <c r="C111">
+        <v>12</v>
+      </c>
+      <c r="D111" t="s">
+        <v>15</v>
+      </c>
+      <c r="E111" t="s">
+        <v>40</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>57</v>
+      </c>
+      <c r="B112">
+        <v>2017</v>
+      </c>
+      <c r="C112">
+        <v>12</v>
+      </c>
+      <c r="D112" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112" t="s">
+        <v>40</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>90</v>
+      </c>
+      <c r="B113">
+        <v>2017</v>
+      </c>
+      <c r="C113">
+        <v>12</v>
+      </c>
+      <c r="D113" t="s">
+        <v>15</v>
+      </c>
+      <c r="E113" t="s">
+        <v>40</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>90</v>
+      </c>
+      <c r="B114">
+        <v>2017</v>
+      </c>
+      <c r="C114">
+        <v>12</v>
+      </c>
+      <c r="D114" t="s">
+        <v>15</v>
+      </c>
+      <c r="E114" t="s">
+        <v>40</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>90</v>
+      </c>
+      <c r="B115">
+        <v>2017</v>
+      </c>
+      <c r="C115">
+        <v>12</v>
+      </c>
+      <c r="D115" t="s">
+        <v>15</v>
+      </c>
+      <c r="E115" t="s">
+        <v>40</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>90</v>
+      </c>
+      <c r="B116">
+        <v>2017</v>
+      </c>
+      <c r="C116">
+        <v>12</v>
+      </c>
+      <c r="D116" t="s">
+        <v>15</v>
+      </c>
+      <c r="E116" t="s">
+        <v>40</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>90</v>
+      </c>
+      <c r="B117">
+        <v>2017</v>
+      </c>
+      <c r="C117">
+        <v>12</v>
+      </c>
+      <c r="D117" t="s">
+        <v>15</v>
+      </c>
+      <c r="E117" t="s">
+        <v>40</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>90</v>
+      </c>
+      <c r="B118">
+        <v>2017</v>
+      </c>
+      <c r="C118">
+        <v>12</v>
+      </c>
+      <c r="D118" t="s">
+        <v>15</v>
+      </c>
+      <c r="E118" t="s">
+        <v>40</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>90</v>
+      </c>
+      <c r="B119">
+        <v>2017</v>
+      </c>
+      <c r="C119">
+        <v>12</v>
+      </c>
+      <c r="D119" t="s">
+        <v>15</v>
+      </c>
+      <c r="E119" t="s">
+        <v>40</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>90</v>
+      </c>
+      <c r="B120">
+        <v>2017</v>
+      </c>
+      <c r="C120">
+        <v>12</v>
+      </c>
+      <c r="D120" t="s">
+        <v>15</v>
+      </c>
+      <c r="E120" t="s">
+        <v>40</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>90</v>
+      </c>
+      <c r="B121">
+        <v>2017</v>
+      </c>
+      <c r="C121">
+        <v>12</v>
+      </c>
+      <c r="D121" t="s">
+        <v>15</v>
+      </c>
+      <c r="E121" t="s">
+        <v>40</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>90</v>
+      </c>
+      <c r="B122">
+        <v>2017</v>
+      </c>
+      <c r="C122">
+        <v>12</v>
+      </c>
+      <c r="D122" t="s">
+        <v>15</v>
+      </c>
+      <c r="E122" t="s">
+        <v>40</v>
+      </c>
+      <c r="F122" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>90</v>
+      </c>
+      <c r="B123">
+        <v>2017</v>
+      </c>
+      <c r="C123">
+        <v>12</v>
+      </c>
+      <c r="D123" t="s">
+        <v>15</v>
+      </c>
+      <c r="E123" t="s">
+        <v>40</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>90</v>
+      </c>
+      <c r="B124">
+        <v>2017</v>
+      </c>
+      <c r="C124">
+        <v>12</v>
+      </c>
+      <c r="D124" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" t="s">
+        <v>40</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>90</v>
+      </c>
+      <c r="B125">
+        <v>2017</v>
+      </c>
+      <c r="C125">
+        <v>12</v>
+      </c>
+      <c r="D125" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" t="s">
+        <v>40</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>90</v>
+      </c>
+      <c r="B126">
+        <v>2017</v>
+      </c>
+      <c r="C126">
+        <v>12</v>
+      </c>
+      <c r="D126" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" t="s">
+        <v>40</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>90</v>
+      </c>
+      <c r="B127">
+        <v>2017</v>
+      </c>
+      <c r="C127">
+        <v>12</v>
+      </c>
+      <c r="D127" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" t="s">
+        <v>40</v>
+      </c>
+      <c r="F127" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>90</v>
+      </c>
+      <c r="B128">
+        <v>2017</v>
+      </c>
+      <c r="C128">
+        <v>12</v>
+      </c>
+      <c r="D128" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" t="s">
+        <v>40</v>
+      </c>
+      <c r="F128" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>90</v>
+      </c>
+      <c r="B129">
+        <v>2017</v>
+      </c>
+      <c r="C129">
+        <v>12</v>
+      </c>
+      <c r="D129" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" t="s">
+        <v>40</v>
+      </c>
+      <c r="F129" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>90</v>
+      </c>
+      <c r="B130">
+        <v>2017</v>
+      </c>
+      <c r="C130">
+        <v>12</v>
+      </c>
+      <c r="D130" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" t="s">
+        <v>40</v>
+      </c>
+      <c r="F130" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>90</v>
+      </c>
+      <c r="B131">
+        <v>2017</v>
+      </c>
+      <c r="C131">
+        <v>12</v>
+      </c>
+      <c r="D131" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" t="s">
+        <v>40</v>
+      </c>
+      <c r="F131" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>90</v>
+      </c>
+      <c r="B132">
+        <v>2017</v>
+      </c>
+      <c r="C132">
+        <v>12</v>
+      </c>
+      <c r="D132" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" t="s">
+        <v>40</v>
+      </c>
+      <c r="F132" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>90</v>
+      </c>
+      <c r="B133">
+        <v>2017</v>
+      </c>
+      <c r="C133">
+        <v>12</v>
+      </c>
+      <c r="D133" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133" t="s">
+        <v>40</v>
+      </c>
+      <c r="F133" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>90</v>
+      </c>
+      <c r="B134">
+        <v>2017</v>
+      </c>
+      <c r="C134">
+        <v>12</v>
+      </c>
+      <c r="D134" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" t="s">
+        <v>40</v>
+      </c>
+      <c r="F134" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>90</v>
+      </c>
+      <c r="B135">
+        <v>2017</v>
+      </c>
+      <c r="C135">
+        <v>12</v>
+      </c>
+      <c r="D135" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135" t="s">
+        <v>40</v>
+      </c>
+      <c r="F135" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>90</v>
+      </c>
+      <c r="B136">
+        <v>2017</v>
+      </c>
+      <c r="C136">
+        <v>12</v>
+      </c>
+      <c r="D136" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136" t="s">
+        <v>40</v>
+      </c>
+      <c r="F136" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>90</v>
+      </c>
+      <c r="B137">
+        <v>2017</v>
+      </c>
+      <c r="C137">
+        <v>12</v>
+      </c>
+      <c r="D137" t="s">
+        <v>8</v>
+      </c>
+      <c r="E137" t="s">
+        <v>40</v>
+      </c>
+      <c r="F137" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>90</v>
+      </c>
+      <c r="B138">
+        <v>2017</v>
+      </c>
+      <c r="C138">
+        <v>12</v>
+      </c>
+      <c r="D138" t="s">
+        <v>8</v>
+      </c>
+      <c r="E138" t="s">
+        <v>40</v>
+      </c>
+      <c r="F138" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>90</v>
+      </c>
+      <c r="B139">
+        <v>2017</v>
+      </c>
+      <c r="C139">
+        <v>12</v>
+      </c>
+      <c r="D139" t="s">
+        <v>8</v>
+      </c>
+      <c r="E139" t="s">
+        <v>40</v>
+      </c>
+      <c r="F139" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>90</v>
+      </c>
+      <c r="B140">
+        <v>2017</v>
+      </c>
+      <c r="C140">
+        <v>12</v>
+      </c>
+      <c r="D140" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" t="s">
+        <v>40</v>
+      </c>
+      <c r="F140" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>90</v>
+      </c>
+      <c r="B141">
+        <v>2017</v>
+      </c>
+      <c r="C141">
+        <v>12</v>
+      </c>
+      <c r="D141" t="s">
+        <v>162</v>
+      </c>
+      <c r="E141" t="s">
+        <v>40</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>90</v>
+      </c>
+      <c r="B142">
+        <v>2017</v>
+      </c>
+      <c r="C142">
+        <v>12</v>
+      </c>
+      <c r="D142" t="s">
+        <v>162</v>
+      </c>
+      <c r="E142" t="s">
+        <v>21</v>
+      </c>
+      <c r="F142" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>41</v>
+      </c>
+      <c r="B143">
+        <v>2017</v>
+      </c>
+      <c r="C143">
+        <v>12</v>
+      </c>
+      <c r="D143" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143" t="s">
+        <v>21</v>
+      </c>
+      <c r="F143" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>41</v>
+      </c>
+      <c r="B144">
+        <v>2017</v>
+      </c>
+      <c r="C144">
+        <v>12</v>
+      </c>
+      <c r="D144" t="s">
+        <v>15</v>
+      </c>
+      <c r="E144" t="s">
+        <v>40</v>
+      </c>
+      <c r="F144" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>41</v>
+      </c>
+      <c r="B145">
+        <v>2017</v>
+      </c>
+      <c r="C145">
+        <v>12</v>
+      </c>
+      <c r="D145" t="s">
+        <v>15</v>
+      </c>
+      <c r="E145" t="s">
+        <v>40</v>
+      </c>
+      <c r="F145" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>41</v>
+      </c>
+      <c r="B146">
+        <v>2017</v>
+      </c>
+      <c r="C146">
+        <v>12</v>
+      </c>
+      <c r="D146" t="s">
+        <v>15</v>
+      </c>
+      <c r="E146" t="s">
+        <v>40</v>
+      </c>
+      <c r="F146" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>41</v>
+      </c>
+      <c r="B147">
+        <v>2017</v>
+      </c>
+      <c r="C147">
+        <v>12</v>
+      </c>
+      <c r="D147" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" t="s">
+        <v>40</v>
+      </c>
+      <c r="F147" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>38</v>
+      </c>
+      <c r="B148">
+        <v>2017</v>
+      </c>
+      <c r="C148">
+        <v>12</v>
+      </c>
+      <c r="D148" t="s">
+        <v>15</v>
+      </c>
+      <c r="E148" t="s">
+        <v>21</v>
+      </c>
+      <c r="F148" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>38</v>
+      </c>
+      <c r="B149">
+        <v>2017</v>
+      </c>
+      <c r="C149">
+        <v>12</v>
+      </c>
+      <c r="D149" t="s">
+        <v>15</v>
+      </c>
+      <c r="E149" t="s">
+        <v>40</v>
+      </c>
+      <c r="F149" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>38</v>
+      </c>
+      <c r="B150">
+        <v>2017</v>
+      </c>
+      <c r="C150">
+        <v>12</v>
+      </c>
+      <c r="D150" t="s">
+        <v>15</v>
+      </c>
+      <c r="E150" t="s">
+        <v>40</v>
+      </c>
+      <c r="F150" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>38</v>
+      </c>
+      <c r="B151">
+        <v>2017</v>
+      </c>
+      <c r="C151">
+        <v>12</v>
+      </c>
+      <c r="D151" t="s">
+        <v>15</v>
+      </c>
+      <c r="E151" t="s">
+        <v>40</v>
+      </c>
+      <c r="F151" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>38</v>
+      </c>
+      <c r="B152">
+        <v>2017</v>
+      </c>
+      <c r="C152">
+        <v>12</v>
+      </c>
+      <c r="D152" t="s">
+        <v>15</v>
+      </c>
+      <c r="E152" t="s">
+        <v>40</v>
+      </c>
+      <c r="F152" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>38</v>
+      </c>
+      <c r="B153">
+        <v>2017</v>
+      </c>
+      <c r="C153">
+        <v>12</v>
+      </c>
+      <c r="D153" t="s">
+        <v>15</v>
+      </c>
+      <c r="E153" t="s">
+        <v>40</v>
+      </c>
+      <c r="F153" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2847,6 +4047,32 @@
     <hyperlink ref="F99" r:id="rId97" xr:uid="{88BD12A1-9F16-437A-8628-00E913A3824F}"/>
     <hyperlink ref="F100" r:id="rId98" xr:uid="{D2612746-B977-4D18-89A2-9B318417785B}"/>
     <hyperlink ref="F101" r:id="rId99" xr:uid="{906F1653-D166-4689-9E77-BA736B9A224A}"/>
+    <hyperlink ref="F102" r:id="rId100" xr:uid="{7720AFBE-EF2D-47FB-A5C5-9B1FE6308204}"/>
+    <hyperlink ref="F103" r:id="rId101" xr:uid="{CF1FA6B2-1C15-43F7-9D5F-E909C7DFCD7B}"/>
+    <hyperlink ref="F104" r:id="rId102" xr:uid="{FD81E693-79CA-4B6B-B055-3B9FD79C8FF1}"/>
+    <hyperlink ref="F105" r:id="rId103" xr:uid="{A3FE253B-9596-4449-AA97-DEE96A8EA300}"/>
+    <hyperlink ref="F106" r:id="rId104" xr:uid="{2CB15426-1D0E-4B59-812A-97D6C515D707}"/>
+    <hyperlink ref="F107" r:id="rId105" xr:uid="{FE68DCE4-DCD5-4CB8-AA03-30C5ECF7B732}"/>
+    <hyperlink ref="F108" r:id="rId106" xr:uid="{70CE5103-7867-4764-BBA2-E72FA3ACF11A}"/>
+    <hyperlink ref="F109" r:id="rId107" xr:uid="{CC1A127D-1E2F-4F71-A393-2DD053F3F605}"/>
+    <hyperlink ref="F110" r:id="rId108" xr:uid="{E290F1A9-97E4-432A-8709-EE15B3625B92}"/>
+    <hyperlink ref="F111" r:id="rId109" xr:uid="{0077EFC4-98C9-49FE-ADD8-7DFD4880CEA3}"/>
+    <hyperlink ref="F112" r:id="rId110" xr:uid="{01221289-AD31-421B-BE00-CD14FC56EFA3}"/>
+    <hyperlink ref="F113" r:id="rId111" xr:uid="{509EA3FE-5637-4C47-9417-A3D6E8C8860B}"/>
+    <hyperlink ref="F114" r:id="rId112" xr:uid="{ADB56528-91EB-42B7-AB21-6FFC84EE571C}"/>
+    <hyperlink ref="F115" r:id="rId113" xr:uid="{2D52723F-2839-48F0-82D5-53E799CC5612}"/>
+    <hyperlink ref="F116" r:id="rId114" xr:uid="{6D72C74E-6A00-43E4-A39D-BB9046463BAA}"/>
+    <hyperlink ref="F117" r:id="rId115" xr:uid="{1A076A39-34E9-48EA-96CE-8F43752036D4}"/>
+    <hyperlink ref="F118" r:id="rId116" xr:uid="{063416AE-9129-47AB-A74D-9BE3D9B45A60}"/>
+    <hyperlink ref="F119" r:id="rId117" xr:uid="{457EDF6C-686C-4649-9D52-FF22F61B924C}"/>
+    <hyperlink ref="F120" r:id="rId118" xr:uid="{C57B2576-8722-436D-9A62-5716A48DF78A}"/>
+    <hyperlink ref="F121" r:id="rId119" xr:uid="{783FEA51-F3CF-4C63-BB85-8C3EA5082446}"/>
+    <hyperlink ref="F123" r:id="rId120" xr:uid="{281CF9EB-BA09-48AD-917D-A5F355ABC7A3}"/>
+    <hyperlink ref="F124" r:id="rId121" xr:uid="{8B6370F4-A21D-476B-88FA-EC8B287E4C1F}"/>
+    <hyperlink ref="F125" r:id="rId122" xr:uid="{9409995D-EBC2-474B-B12A-B6880CCB1C79}"/>
+    <hyperlink ref="F126" r:id="rId123" xr:uid="{27577B03-D7E2-4AC2-A295-6FA4FEC07C80}"/>
+    <hyperlink ref="F141" r:id="rId124" xr:uid="{FEA82B65-F692-4B64-A7B6-96C167030B4B}"/>
+    <hyperlink ref="F148" r:id="rId125" xr:uid="{F8AAA501-9094-4BB2-B91B-76944DF646E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add JAS Dec 2017
</commit_message>
<xml_diff>
--- a/journal_URL.xlsx
+++ b/journal_URL.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="193">
   <si>
     <t>journal</t>
   </si>
@@ -544,6 +544,60 @@
   </si>
   <si>
     <t>http://www.sciencedirect.com/science/article/pii/S0022030217309219</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5290</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5420</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5430</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5439</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5447</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5455</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5466</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5474</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5485</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5507</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5516</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5547</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5563</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5573</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5584</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5597</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5606</t>
+  </si>
+  <si>
+    <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5617</t>
   </si>
 </sst>
 </file>
@@ -872,11 +926,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F153"/>
+  <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E159" sqref="E159"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3944,6 +3998,366 @@
       </c>
       <c r="F153" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>1</v>
+      </c>
+      <c r="B154">
+        <v>2017</v>
+      </c>
+      <c r="C154">
+        <v>12</v>
+      </c>
+      <c r="D154" t="s">
+        <v>15</v>
+      </c>
+      <c r="E154" t="s">
+        <v>40</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>1</v>
+      </c>
+      <c r="B155">
+        <v>2017</v>
+      </c>
+      <c r="C155">
+        <v>12</v>
+      </c>
+      <c r="D155" t="s">
+        <v>8</v>
+      </c>
+      <c r="E155" t="s">
+        <v>40</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>1</v>
+      </c>
+      <c r="B156">
+        <v>2017</v>
+      </c>
+      <c r="C156">
+        <v>12</v>
+      </c>
+      <c r="D156" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" t="s">
+        <v>40</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>1</v>
+      </c>
+      <c r="B157">
+        <v>2017</v>
+      </c>
+      <c r="C157">
+        <v>12</v>
+      </c>
+      <c r="D157" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" t="s">
+        <v>40</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>1</v>
+      </c>
+      <c r="B158">
+        <v>2017</v>
+      </c>
+      <c r="C158">
+        <v>12</v>
+      </c>
+      <c r="D158" t="s">
+        <v>8</v>
+      </c>
+      <c r="E158" t="s">
+        <v>40</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>1</v>
+      </c>
+      <c r="B159">
+        <v>2017</v>
+      </c>
+      <c r="C159">
+        <v>12</v>
+      </c>
+      <c r="D159" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" t="s">
+        <v>40</v>
+      </c>
+      <c r="F159" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>1</v>
+      </c>
+      <c r="B160">
+        <v>2017</v>
+      </c>
+      <c r="C160">
+        <v>12</v>
+      </c>
+      <c r="D160" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" t="s">
+        <v>40</v>
+      </c>
+      <c r="F160" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>1</v>
+      </c>
+      <c r="B161">
+        <v>2017</v>
+      </c>
+      <c r="C161">
+        <v>12</v>
+      </c>
+      <c r="D161" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" t="s">
+        <v>40</v>
+      </c>
+      <c r="F161" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>1</v>
+      </c>
+      <c r="B162">
+        <v>2017</v>
+      </c>
+      <c r="C162">
+        <v>12</v>
+      </c>
+      <c r="D162" t="s">
+        <v>8</v>
+      </c>
+      <c r="E162" t="s">
+        <v>40</v>
+      </c>
+      <c r="F162" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>1</v>
+      </c>
+      <c r="B163">
+        <v>2017</v>
+      </c>
+      <c r="C163">
+        <v>12</v>
+      </c>
+      <c r="D163" t="s">
+        <v>8</v>
+      </c>
+      <c r="E163" t="s">
+        <v>40</v>
+      </c>
+      <c r="F163" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>1</v>
+      </c>
+      <c r="B164">
+        <v>2017</v>
+      </c>
+      <c r="C164">
+        <v>12</v>
+      </c>
+      <c r="D164" t="s">
+        <v>8</v>
+      </c>
+      <c r="E164" t="s">
+        <v>40</v>
+      </c>
+      <c r="F164" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>1</v>
+      </c>
+      <c r="B165">
+        <v>2017</v>
+      </c>
+      <c r="C165">
+        <v>12</v>
+      </c>
+      <c r="D165" t="s">
+        <v>15</v>
+      </c>
+      <c r="E165" t="s">
+        <v>40</v>
+      </c>
+      <c r="F165" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>1</v>
+      </c>
+      <c r="B166">
+        <v>2017</v>
+      </c>
+      <c r="C166">
+        <v>12</v>
+      </c>
+      <c r="D166" t="s">
+        <v>15</v>
+      </c>
+      <c r="E166" t="s">
+        <v>40</v>
+      </c>
+      <c r="F166" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>1</v>
+      </c>
+      <c r="B167">
+        <v>2017</v>
+      </c>
+      <c r="C167">
+        <v>12</v>
+      </c>
+      <c r="D167" t="s">
+        <v>15</v>
+      </c>
+      <c r="E167" t="s">
+        <v>40</v>
+      </c>
+      <c r="F167" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>1</v>
+      </c>
+      <c r="B168">
+        <v>2017</v>
+      </c>
+      <c r="C168">
+        <v>12</v>
+      </c>
+      <c r="D168" t="s">
+        <v>15</v>
+      </c>
+      <c r="E168" t="s">
+        <v>40</v>
+      </c>
+      <c r="F168" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>1</v>
+      </c>
+      <c r="B169">
+        <v>2017</v>
+      </c>
+      <c r="C169">
+        <v>12</v>
+      </c>
+      <c r="D169" t="s">
+        <v>15</v>
+      </c>
+      <c r="E169" t="s">
+        <v>40</v>
+      </c>
+      <c r="F169" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>1</v>
+      </c>
+      <c r="B170">
+        <v>2017</v>
+      </c>
+      <c r="C170">
+        <v>12</v>
+      </c>
+      <c r="D170" t="s">
+        <v>15</v>
+      </c>
+      <c r="E170" t="s">
+        <v>40</v>
+      </c>
+      <c r="F170" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>1</v>
+      </c>
+      <c r="B171">
+        <v>2017</v>
+      </c>
+      <c r="C171">
+        <v>12</v>
+      </c>
+      <c r="D171" t="s">
+        <v>15</v>
+      </c>
+      <c r="E171" t="s">
+        <v>40</v>
+      </c>
+      <c r="F171" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4073,6 +4487,11 @@
     <hyperlink ref="F126" r:id="rId123" xr:uid="{27577B03-D7E2-4AC2-A295-6FA4FEC07C80}"/>
     <hyperlink ref="F141" r:id="rId124" xr:uid="{FEA82B65-F692-4B64-A7B6-96C167030B4B}"/>
     <hyperlink ref="F148" r:id="rId125" xr:uid="{F8AAA501-9094-4BB2-B91B-76944DF646E5}"/>
+    <hyperlink ref="F154" r:id="rId126" xr:uid="{B9459A9E-36B4-4701-8BFF-58F3348A09D1}"/>
+    <hyperlink ref="F155" r:id="rId127" xr:uid="{D6FAF2CD-864F-4037-87F5-51D3A9F77E1E}"/>
+    <hyperlink ref="F156" r:id="rId128" xr:uid="{48323B38-D479-46AC-B219-915FBB77DFD8}"/>
+    <hyperlink ref="F157" r:id="rId129" xr:uid="{C6A97135-FE75-4E74-9E08-30F3469A9E3C}"/>
+    <hyperlink ref="F158" r:id="rId130" xr:uid="{CC0C1FB7-F9E6-4F27-A344-9D3DC76C05F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
publish AJNR Dec 2017
</commit_message>
<xml_diff>
--- a/journal_URL.xlsx
+++ b/journal_URL.xlsx
@@ -929,13 +929,13 @@
   <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D170" sqref="D170"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F147" sqref="F147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
add scrapping codes for JAS (Oxford ver.)
</commit_message>
<xml_diff>
--- a/journal_URL.xlsx
+++ b/journal_URL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -929,8 +929,8 @@
   <dimension ref="A1:F171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F147" sqref="F147"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A172" sqref="A172:XFD172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add URL of Jan 2018
</commit_message>
<xml_diff>
--- a/journal_URL.xlsx
+++ b/journal_URL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="278">
   <si>
     <t>journal</t>
   </si>
@@ -598,6 +598,261 @@
   </si>
   <si>
     <t>https://www.animalsciencepublications.org/publications/jas/articles/95/12/5617</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/0096129AEAEC772A6283EED24D7F92A7</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/10187D2E9BBFF203E179F1E9D82D8D8D</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/FDE9A3166CE7F20D41F8A68070904B0D</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/9933D2406F02B781E7C7039303F9E1C4</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/product/CE7C151B0E8CCA30ECE278C4BFBA08D4</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117314013</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117314104</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117303814</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308775</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117307885</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117307137</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S037784011630877X</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117302353</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117310581</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308167</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117310283</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840116311671</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117307721</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308970</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308398</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117307708</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117303498</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117309690</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117310167</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117309550</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117305357</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23755</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23714</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23907</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23799</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23908</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23823</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23763</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23825</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23856</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23759</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23794</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217310093</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217310081</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S002203021730975X</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309748</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309852</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S002203021730927X</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309384</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309268</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309645</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S002203021730992X</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309906</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309943</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217310068</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309931</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309360</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S002203021731007X</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217310044</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217310111</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309621</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S0022030217309402</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317303372</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S187114131730255X</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317302962</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S1871141317303578</t>
+  </si>
+  <si>
+    <t>http://www.sciencedirect.com/science/article/pii/S187114131730358X</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/84/4565704</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/262/4609698</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/267/4565727</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/88/4565706</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/102/4565708</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/110/4565709</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/118/4565710</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/124/4590020</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/131/4565714</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/140/4565715</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/149/4565716</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/159/4565719</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/167/4565720</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/177/4566212</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/188/4565722</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/196/4609700</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/203/4565723</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/211/4565724</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/219/4590021</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/227/4601754</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/236/4591658</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/247/4565730</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/1/255/4565733</t>
   </si>
 </sst>
 </file>
@@ -642,9 +897,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -926,11 +1182,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F171"/>
+  <dimension ref="A1:F258"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A172" sqref="A172:XFD172"/>
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B259" sqref="B259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4358,6 +4614,1716 @@
       </c>
       <c r="F171" t="s">
         <v>192</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>57</v>
+      </c>
+      <c r="B172">
+        <v>2018</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172" t="s">
+        <v>8</v>
+      </c>
+      <c r="E172" t="s">
+        <v>40</v>
+      </c>
+      <c r="F172" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>57</v>
+      </c>
+      <c r="B173">
+        <v>2018</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+      <c r="D173" t="s">
+        <v>8</v>
+      </c>
+      <c r="E173" t="s">
+        <v>40</v>
+      </c>
+      <c r="F173" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>57</v>
+      </c>
+      <c r="B174">
+        <v>2018</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+      <c r="D174" t="s">
+        <v>8</v>
+      </c>
+      <c r="E174" t="s">
+        <v>40</v>
+      </c>
+      <c r="F174" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>57</v>
+      </c>
+      <c r="B175">
+        <v>2018</v>
+      </c>
+      <c r="C175">
+        <v>1</v>
+      </c>
+      <c r="D175" t="s">
+        <v>15</v>
+      </c>
+      <c r="E175" t="s">
+        <v>40</v>
+      </c>
+      <c r="F175" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>57</v>
+      </c>
+      <c r="B176">
+        <v>2018</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176" t="s">
+        <v>15</v>
+      </c>
+      <c r="E176" t="s">
+        <v>40</v>
+      </c>
+      <c r="F176" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>90</v>
+      </c>
+      <c r="B177">
+        <v>2018</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177" t="s">
+        <v>15</v>
+      </c>
+      <c r="E177" t="s">
+        <v>40</v>
+      </c>
+      <c r="F177" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>90</v>
+      </c>
+      <c r="B178">
+        <v>2018</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+      <c r="D178" t="s">
+        <v>15</v>
+      </c>
+      <c r="E178" t="s">
+        <v>40</v>
+      </c>
+      <c r="F178" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>90</v>
+      </c>
+      <c r="B179">
+        <v>2018</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+      <c r="D179" t="s">
+        <v>15</v>
+      </c>
+      <c r="E179" t="s">
+        <v>40</v>
+      </c>
+      <c r="F179" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>90</v>
+      </c>
+      <c r="B180">
+        <v>2018</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+      <c r="D180" t="s">
+        <v>15</v>
+      </c>
+      <c r="E180" t="s">
+        <v>40</v>
+      </c>
+      <c r="F180" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>90</v>
+      </c>
+      <c r="B181">
+        <v>2018</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181" t="s">
+        <v>15</v>
+      </c>
+      <c r="E181" t="s">
+        <v>40</v>
+      </c>
+      <c r="F181" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>90</v>
+      </c>
+      <c r="B182">
+        <v>2018</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="D182" t="s">
+        <v>15</v>
+      </c>
+      <c r="E182" t="s">
+        <v>40</v>
+      </c>
+      <c r="F182" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>90</v>
+      </c>
+      <c r="B183">
+        <v>2018</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="D183" t="s">
+        <v>15</v>
+      </c>
+      <c r="E183" t="s">
+        <v>40</v>
+      </c>
+      <c r="F183" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>90</v>
+      </c>
+      <c r="B184">
+        <v>2018</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184" t="s">
+        <v>15</v>
+      </c>
+      <c r="E184" t="s">
+        <v>40</v>
+      </c>
+      <c r="F184" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>90</v>
+      </c>
+      <c r="B185">
+        <v>2018</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+      <c r="D185" t="s">
+        <v>15</v>
+      </c>
+      <c r="E185" t="s">
+        <v>40</v>
+      </c>
+      <c r="F185" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>90</v>
+      </c>
+      <c r="B186">
+        <v>2018</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="D186" t="s">
+        <v>8</v>
+      </c>
+      <c r="E186" t="s">
+        <v>40</v>
+      </c>
+      <c r="F186" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>90</v>
+      </c>
+      <c r="B187">
+        <v>2018</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+      <c r="D187" t="s">
+        <v>8</v>
+      </c>
+      <c r="E187" t="s">
+        <v>21</v>
+      </c>
+      <c r="F187" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>90</v>
+      </c>
+      <c r="B188">
+        <v>2018</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+      <c r="D188" t="s">
+        <v>8</v>
+      </c>
+      <c r="E188" t="s">
+        <v>40</v>
+      </c>
+      <c r="F188" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>90</v>
+      </c>
+      <c r="B189">
+        <v>2018</v>
+      </c>
+      <c r="C189">
+        <v>1</v>
+      </c>
+      <c r="D189" t="s">
+        <v>8</v>
+      </c>
+      <c r="E189" t="s">
+        <v>40</v>
+      </c>
+      <c r="F189" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>90</v>
+      </c>
+      <c r="B190">
+        <v>2018</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+      <c r="D190" t="s">
+        <v>8</v>
+      </c>
+      <c r="E190" t="s">
+        <v>40</v>
+      </c>
+      <c r="F190" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>90</v>
+      </c>
+      <c r="B191">
+        <v>2018</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191" t="s">
+        <v>8</v>
+      </c>
+      <c r="E191" t="s">
+        <v>40</v>
+      </c>
+      <c r="F191" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>90</v>
+      </c>
+      <c r="B192">
+        <v>2018</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+      <c r="D192" t="s">
+        <v>8</v>
+      </c>
+      <c r="E192" t="s">
+        <v>40</v>
+      </c>
+      <c r="F192" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>90</v>
+      </c>
+      <c r="B193">
+        <v>2018</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+      <c r="D193" t="s">
+        <v>8</v>
+      </c>
+      <c r="E193" t="s">
+        <v>40</v>
+      </c>
+      <c r="F193" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>90</v>
+      </c>
+      <c r="B194">
+        <v>2018</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="D194" t="s">
+        <v>8</v>
+      </c>
+      <c r="E194" t="s">
+        <v>40</v>
+      </c>
+      <c r="F194" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>90</v>
+      </c>
+      <c r="B195">
+        <v>2018</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+      <c r="D195" t="s">
+        <v>8</v>
+      </c>
+      <c r="E195" t="s">
+        <v>40</v>
+      </c>
+      <c r="F195" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>90</v>
+      </c>
+      <c r="B196">
+        <v>2018</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="D196" t="s">
+        <v>8</v>
+      </c>
+      <c r="E196" t="s">
+        <v>40</v>
+      </c>
+      <c r="F196" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>90</v>
+      </c>
+      <c r="B197">
+        <v>2018</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="D197" t="s">
+        <v>8</v>
+      </c>
+      <c r="E197" t="s">
+        <v>40</v>
+      </c>
+      <c r="F197" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>41</v>
+      </c>
+      <c r="B198">
+        <v>2018</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+      <c r="D198" t="s">
+        <v>15</v>
+      </c>
+      <c r="E198" t="s">
+        <v>40</v>
+      </c>
+      <c r="F198" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>41</v>
+      </c>
+      <c r="B199">
+        <v>2018</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+      <c r="D199" t="s">
+        <v>15</v>
+      </c>
+      <c r="E199" t="s">
+        <v>40</v>
+      </c>
+      <c r="F199" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>41</v>
+      </c>
+      <c r="B200">
+        <v>2018</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+      <c r="D200" t="s">
+        <v>15</v>
+      </c>
+      <c r="E200" t="s">
+        <v>40</v>
+      </c>
+      <c r="F200" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>41</v>
+      </c>
+      <c r="B201">
+        <v>2018</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+      <c r="D201" t="s">
+        <v>15</v>
+      </c>
+      <c r="E201" t="s">
+        <v>40</v>
+      </c>
+      <c r="F201" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>41</v>
+      </c>
+      <c r="B202">
+        <v>2018</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+      <c r="D202" t="s">
+        <v>15</v>
+      </c>
+      <c r="E202" t="s">
+        <v>40</v>
+      </c>
+      <c r="F202" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>41</v>
+      </c>
+      <c r="B203">
+        <v>2018</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+      <c r="D203" t="s">
+        <v>15</v>
+      </c>
+      <c r="E203" t="s">
+        <v>40</v>
+      </c>
+      <c r="F203" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>41</v>
+      </c>
+      <c r="B204">
+        <v>2018</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+      <c r="D204" t="s">
+        <v>8</v>
+      </c>
+      <c r="E204" t="s">
+        <v>40</v>
+      </c>
+      <c r="F204" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>41</v>
+      </c>
+      <c r="B205">
+        <v>2018</v>
+      </c>
+      <c r="C205">
+        <v>1</v>
+      </c>
+      <c r="D205" t="s">
+        <v>8</v>
+      </c>
+      <c r="E205" t="s">
+        <v>40</v>
+      </c>
+      <c r="F205" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>41</v>
+      </c>
+      <c r="B206">
+        <v>2018</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+      <c r="D206" t="s">
+        <v>8</v>
+      </c>
+      <c r="E206" t="s">
+        <v>40</v>
+      </c>
+      <c r="F206" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>41</v>
+      </c>
+      <c r="B207">
+        <v>2018</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+      <c r="D207" t="s">
+        <v>8</v>
+      </c>
+      <c r="E207" t="s">
+        <v>40</v>
+      </c>
+      <c r="F207" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>41</v>
+      </c>
+      <c r="B208">
+        <v>2018</v>
+      </c>
+      <c r="C208">
+        <v>1</v>
+      </c>
+      <c r="D208" t="s">
+        <v>8</v>
+      </c>
+      <c r="E208" t="s">
+        <v>40</v>
+      </c>
+      <c r="F208" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>38</v>
+      </c>
+      <c r="B209">
+        <v>2018</v>
+      </c>
+      <c r="C209">
+        <v>1</v>
+      </c>
+      <c r="D209" t="s">
+        <v>15</v>
+      </c>
+      <c r="E209" t="s">
+        <v>40</v>
+      </c>
+      <c r="F209" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>38</v>
+      </c>
+      <c r="B210">
+        <v>2018</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+      <c r="D210" t="s">
+        <v>15</v>
+      </c>
+      <c r="E210" t="s">
+        <v>40</v>
+      </c>
+      <c r="F210" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>38</v>
+      </c>
+      <c r="B211">
+        <v>2018</v>
+      </c>
+      <c r="C211">
+        <v>1</v>
+      </c>
+      <c r="D211" t="s">
+        <v>15</v>
+      </c>
+      <c r="E211" t="s">
+        <v>40</v>
+      </c>
+      <c r="F211" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>38</v>
+      </c>
+      <c r="B212">
+        <v>2018</v>
+      </c>
+      <c r="C212">
+        <v>1</v>
+      </c>
+      <c r="D212" t="s">
+        <v>15</v>
+      </c>
+      <c r="E212" t="s">
+        <v>40</v>
+      </c>
+      <c r="F212" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>38</v>
+      </c>
+      <c r="B213">
+        <v>2018</v>
+      </c>
+      <c r="C213">
+        <v>1</v>
+      </c>
+      <c r="D213" t="s">
+        <v>15</v>
+      </c>
+      <c r="E213" t="s">
+        <v>40</v>
+      </c>
+      <c r="F213" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>38</v>
+      </c>
+      <c r="B214">
+        <v>2018</v>
+      </c>
+      <c r="C214">
+        <v>1</v>
+      </c>
+      <c r="D214" t="s">
+        <v>15</v>
+      </c>
+      <c r="E214" t="s">
+        <v>40</v>
+      </c>
+      <c r="F214" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>38</v>
+      </c>
+      <c r="B215">
+        <v>2018</v>
+      </c>
+      <c r="C215">
+        <v>1</v>
+      </c>
+      <c r="D215" t="s">
+        <v>15</v>
+      </c>
+      <c r="E215" t="s">
+        <v>40</v>
+      </c>
+      <c r="F215" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>38</v>
+      </c>
+      <c r="B216">
+        <v>2018</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+      <c r="D216" t="s">
+        <v>15</v>
+      </c>
+      <c r="E216" t="s">
+        <v>40</v>
+      </c>
+      <c r="F216" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>38</v>
+      </c>
+      <c r="B217">
+        <v>2018</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+      <c r="D217" t="s">
+        <v>15</v>
+      </c>
+      <c r="E217" t="s">
+        <v>40</v>
+      </c>
+      <c r="F217" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>38</v>
+      </c>
+      <c r="B218">
+        <v>2018</v>
+      </c>
+      <c r="C218">
+        <v>1</v>
+      </c>
+      <c r="D218" t="s">
+        <v>15</v>
+      </c>
+      <c r="E218" t="s">
+        <v>40</v>
+      </c>
+      <c r="F218" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>38</v>
+      </c>
+      <c r="B219">
+        <v>2018</v>
+      </c>
+      <c r="C219">
+        <v>1</v>
+      </c>
+      <c r="D219" t="s">
+        <v>15</v>
+      </c>
+      <c r="E219" t="s">
+        <v>40</v>
+      </c>
+      <c r="F219" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>38</v>
+      </c>
+      <c r="B220">
+        <v>2018</v>
+      </c>
+      <c r="C220">
+        <v>1</v>
+      </c>
+      <c r="D220" t="s">
+        <v>15</v>
+      </c>
+      <c r="E220" t="s">
+        <v>40</v>
+      </c>
+      <c r="F220" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>38</v>
+      </c>
+      <c r="B221">
+        <v>2018</v>
+      </c>
+      <c r="C221">
+        <v>1</v>
+      </c>
+      <c r="D221" t="s">
+        <v>15</v>
+      </c>
+      <c r="E221" t="s">
+        <v>40</v>
+      </c>
+      <c r="F221" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>38</v>
+      </c>
+      <c r="B222">
+        <v>2018</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+      <c r="D222" t="s">
+        <v>15</v>
+      </c>
+      <c r="E222" t="s">
+        <v>40</v>
+      </c>
+      <c r="F222" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>38</v>
+      </c>
+      <c r="B223">
+        <v>2018</v>
+      </c>
+      <c r="C223">
+        <v>1</v>
+      </c>
+      <c r="D223" t="s">
+        <v>15</v>
+      </c>
+      <c r="E223" t="s">
+        <v>40</v>
+      </c>
+      <c r="F223" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>38</v>
+      </c>
+      <c r="B224">
+        <v>2018</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+      <c r="D224" t="s">
+        <v>15</v>
+      </c>
+      <c r="E224" t="s">
+        <v>40</v>
+      </c>
+      <c r="F224" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>38</v>
+      </c>
+      <c r="B225">
+        <v>2018</v>
+      </c>
+      <c r="C225">
+        <v>1</v>
+      </c>
+      <c r="D225" t="s">
+        <v>15</v>
+      </c>
+      <c r="E225" t="s">
+        <v>40</v>
+      </c>
+      <c r="F225" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>38</v>
+      </c>
+      <c r="B226">
+        <v>2018</v>
+      </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
+      <c r="D226" t="s">
+        <v>15</v>
+      </c>
+      <c r="E226" t="s">
+        <v>40</v>
+      </c>
+      <c r="F226" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>38</v>
+      </c>
+      <c r="B227">
+        <v>2018</v>
+      </c>
+      <c r="C227">
+        <v>1</v>
+      </c>
+      <c r="D227" t="s">
+        <v>15</v>
+      </c>
+      <c r="E227" t="s">
+        <v>40</v>
+      </c>
+      <c r="F227" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>38</v>
+      </c>
+      <c r="B228">
+        <v>2018</v>
+      </c>
+      <c r="C228">
+        <v>1</v>
+      </c>
+      <c r="D228" t="s">
+        <v>15</v>
+      </c>
+      <c r="E228" t="s">
+        <v>40</v>
+      </c>
+      <c r="F228" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>91</v>
+      </c>
+      <c r="B229">
+        <v>2018</v>
+      </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+      <c r="D229" t="s">
+        <v>15</v>
+      </c>
+      <c r="E229" t="s">
+        <v>40</v>
+      </c>
+      <c r="F229" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>91</v>
+      </c>
+      <c r="B230">
+        <v>2018</v>
+      </c>
+      <c r="C230">
+        <v>1</v>
+      </c>
+      <c r="D230" t="s">
+        <v>15</v>
+      </c>
+      <c r="E230" t="s">
+        <v>40</v>
+      </c>
+      <c r="F230" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>91</v>
+      </c>
+      <c r="B231">
+        <v>2018</v>
+      </c>
+      <c r="C231">
+        <v>1</v>
+      </c>
+      <c r="D231" t="s">
+        <v>8</v>
+      </c>
+      <c r="E231" t="s">
+        <v>40</v>
+      </c>
+      <c r="F231" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>91</v>
+      </c>
+      <c r="B232">
+        <v>2018</v>
+      </c>
+      <c r="C232">
+        <v>1</v>
+      </c>
+      <c r="D232" t="s">
+        <v>8</v>
+      </c>
+      <c r="E232" t="s">
+        <v>40</v>
+      </c>
+      <c r="F232" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>91</v>
+      </c>
+      <c r="B233">
+        <v>2018</v>
+      </c>
+      <c r="C233">
+        <v>1</v>
+      </c>
+      <c r="D233" t="s">
+        <v>8</v>
+      </c>
+      <c r="E233" t="s">
+        <v>40</v>
+      </c>
+      <c r="F233" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>66</v>
+      </c>
+      <c r="B234">
+        <v>2018</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+      <c r="D234" t="s">
+        <v>8</v>
+      </c>
+      <c r="E234" t="s">
+        <v>21</v>
+      </c>
+      <c r="F234" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>66</v>
+      </c>
+      <c r="B235">
+        <v>2018</v>
+      </c>
+      <c r="C235">
+        <v>1</v>
+      </c>
+      <c r="D235" t="s">
+        <v>8</v>
+      </c>
+      <c r="E235" t="s">
+        <v>40</v>
+      </c>
+      <c r="F235" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>66</v>
+      </c>
+      <c r="B236">
+        <v>2018</v>
+      </c>
+      <c r="C236">
+        <v>1</v>
+      </c>
+      <c r="D236" t="s">
+        <v>8</v>
+      </c>
+      <c r="E236" t="s">
+        <v>40</v>
+      </c>
+      <c r="F236" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>66</v>
+      </c>
+      <c r="B237">
+        <v>2018</v>
+      </c>
+      <c r="C237">
+        <v>1</v>
+      </c>
+      <c r="D237" t="s">
+        <v>8</v>
+      </c>
+      <c r="E237" t="s">
+        <v>40</v>
+      </c>
+      <c r="F237" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>66</v>
+      </c>
+      <c r="B238">
+        <v>2018</v>
+      </c>
+      <c r="C238">
+        <v>1</v>
+      </c>
+      <c r="D238" t="s">
+        <v>8</v>
+      </c>
+      <c r="E238" t="s">
+        <v>40</v>
+      </c>
+      <c r="F238" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>66</v>
+      </c>
+      <c r="B239">
+        <v>2018</v>
+      </c>
+      <c r="C239">
+        <v>1</v>
+      </c>
+      <c r="D239" t="s">
+        <v>8</v>
+      </c>
+      <c r="E239" t="s">
+        <v>40</v>
+      </c>
+      <c r="F239" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>66</v>
+      </c>
+      <c r="B240">
+        <v>2018</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240" t="s">
+        <v>8</v>
+      </c>
+      <c r="E240" t="s">
+        <v>40</v>
+      </c>
+      <c r="F240" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>66</v>
+      </c>
+      <c r="B241">
+        <v>2018</v>
+      </c>
+      <c r="C241">
+        <v>1</v>
+      </c>
+      <c r="D241" t="s">
+        <v>8</v>
+      </c>
+      <c r="E241" t="s">
+        <v>40</v>
+      </c>
+      <c r="F241" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>66</v>
+      </c>
+      <c r="B242">
+        <v>2018</v>
+      </c>
+      <c r="C242">
+        <v>1</v>
+      </c>
+      <c r="D242" t="s">
+        <v>8</v>
+      </c>
+      <c r="E242" t="s">
+        <v>40</v>
+      </c>
+      <c r="F242" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>66</v>
+      </c>
+      <c r="B243">
+        <v>2018</v>
+      </c>
+      <c r="C243">
+        <v>1</v>
+      </c>
+      <c r="D243" t="s">
+        <v>8</v>
+      </c>
+      <c r="E243" t="s">
+        <v>40</v>
+      </c>
+      <c r="F243" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>66</v>
+      </c>
+      <c r="B244">
+        <v>2018</v>
+      </c>
+      <c r="C244">
+        <v>1</v>
+      </c>
+      <c r="D244" t="s">
+        <v>8</v>
+      </c>
+      <c r="E244" t="s">
+        <v>40</v>
+      </c>
+      <c r="F244" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>66</v>
+      </c>
+      <c r="B245">
+        <v>2018</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
+      <c r="D245" t="s">
+        <v>8</v>
+      </c>
+      <c r="E245" t="s">
+        <v>40</v>
+      </c>
+      <c r="F245" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>66</v>
+      </c>
+      <c r="B246">
+        <v>2018</v>
+      </c>
+      <c r="C246">
+        <v>1</v>
+      </c>
+      <c r="D246" t="s">
+        <v>8</v>
+      </c>
+      <c r="E246" t="s">
+        <v>40</v>
+      </c>
+      <c r="F246" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>66</v>
+      </c>
+      <c r="B247">
+        <v>2018</v>
+      </c>
+      <c r="C247">
+        <v>1</v>
+      </c>
+      <c r="D247" t="s">
+        <v>8</v>
+      </c>
+      <c r="E247" t="s">
+        <v>40</v>
+      </c>
+      <c r="F247" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>66</v>
+      </c>
+      <c r="B248">
+        <v>2018</v>
+      </c>
+      <c r="C248">
+        <v>1</v>
+      </c>
+      <c r="D248" t="s">
+        <v>8</v>
+      </c>
+      <c r="E248" t="s">
+        <v>40</v>
+      </c>
+      <c r="F248" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>66</v>
+      </c>
+      <c r="B249">
+        <v>2018</v>
+      </c>
+      <c r="C249">
+        <v>1</v>
+      </c>
+      <c r="D249" t="s">
+        <v>8</v>
+      </c>
+      <c r="E249" t="s">
+        <v>40</v>
+      </c>
+      <c r="F249" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>66</v>
+      </c>
+      <c r="B250">
+        <v>2018</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
+      <c r="D250" t="s">
+        <v>8</v>
+      </c>
+      <c r="E250" t="s">
+        <v>40</v>
+      </c>
+      <c r="F250" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>66</v>
+      </c>
+      <c r="B251">
+        <v>2018</v>
+      </c>
+      <c r="C251">
+        <v>1</v>
+      </c>
+      <c r="D251" t="s">
+        <v>8</v>
+      </c>
+      <c r="E251" t="s">
+        <v>40</v>
+      </c>
+      <c r="F251" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>66</v>
+      </c>
+      <c r="B252">
+        <v>2018</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+      <c r="D252" t="s">
+        <v>8</v>
+      </c>
+      <c r="E252" t="s">
+        <v>40</v>
+      </c>
+      <c r="F252" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>66</v>
+      </c>
+      <c r="B253">
+        <v>2018</v>
+      </c>
+      <c r="C253">
+        <v>1</v>
+      </c>
+      <c r="D253" t="s">
+        <v>8</v>
+      </c>
+      <c r="E253" t="s">
+        <v>40</v>
+      </c>
+      <c r="F253" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>66</v>
+      </c>
+      <c r="B254">
+        <v>2018</v>
+      </c>
+      <c r="C254">
+        <v>1</v>
+      </c>
+      <c r="D254" t="s">
+        <v>8</v>
+      </c>
+      <c r="E254" t="s">
+        <v>40</v>
+      </c>
+      <c r="F254" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>66</v>
+      </c>
+      <c r="B255">
+        <v>2018</v>
+      </c>
+      <c r="C255">
+        <v>1</v>
+      </c>
+      <c r="D255" t="s">
+        <v>8</v>
+      </c>
+      <c r="E255" t="s">
+        <v>40</v>
+      </c>
+      <c r="F255" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>66</v>
+      </c>
+      <c r="B256">
+        <v>2018</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
+      <c r="D256" t="s">
+        <v>8</v>
+      </c>
+      <c r="E256" t="s">
+        <v>40</v>
+      </c>
+      <c r="F256" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Jan 2018 data
</commit_message>
<xml_diff>
--- a/journal_URL.xlsx
+++ b/journal_URL.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="294">
   <si>
     <t>journal</t>
   </si>
@@ -853,6 +853,54 @@
   </si>
   <si>
     <t>https://academic.oup.com/ps/article/97/1/255/4565733</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/98/4844089</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/168/4844098</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/181/4827713</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/194/4827625</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/206/4824921</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/215/4844080</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/225/4824872</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/273/4827718</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/284/4827785</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/293/4827629</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/306/4844085</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/318/4825262</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/331/4825179</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/343/4818648</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/354/4818673</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/1/364/4818649</t>
   </si>
 </sst>
 </file>
@@ -1182,11 +1230,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F258"/>
+  <dimension ref="A1:F272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B259" sqref="B259"/>
+      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D279" sqref="D279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6032,7 +6080,7 @@
       <c r="E242" t="s">
         <v>40</v>
       </c>
-      <c r="F242" t="s">
+      <c r="F242" s="1" t="s">
         <v>263</v>
       </c>
     </row>
@@ -6316,14 +6364,324 @@
         <v>277</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B257">
+        <v>2018</v>
+      </c>
+      <c r="C257">
+        <v>1</v>
+      </c>
+      <c r="D257" t="s">
+        <v>8</v>
+      </c>
+      <c r="E257" t="s">
+        <v>40</v>
+      </c>
+      <c r="F257" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>1</v>
+      </c>
+      <c r="B258">
+        <v>2018</v>
+      </c>
+      <c r="C258">
+        <v>1</v>
+      </c>
+      <c r="D258" t="s">
+        <v>8</v>
+      </c>
+      <c r="E258" t="s">
+        <v>40</v>
+      </c>
+      <c r="F258" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>1</v>
+      </c>
+      <c r="B259">
+        <v>2018</v>
+      </c>
+      <c r="C259">
+        <v>1</v>
+      </c>
+      <c r="D259" t="s">
+        <v>8</v>
+      </c>
+      <c r="E259" t="s">
+        <v>40</v>
+      </c>
+      <c r="F259" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>1</v>
+      </c>
+      <c r="B260">
+        <v>2018</v>
+      </c>
+      <c r="C260">
+        <v>1</v>
+      </c>
+      <c r="D260" t="s">
+        <v>8</v>
+      </c>
+      <c r="E260" t="s">
+        <v>40</v>
+      </c>
+      <c r="F260" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>1</v>
+      </c>
+      <c r="B261">
+        <v>2018</v>
+      </c>
+      <c r="C261">
+        <v>1</v>
+      </c>
+      <c r="D261" t="s">
+        <v>8</v>
+      </c>
+      <c r="E261" t="s">
+        <v>40</v>
+      </c>
+      <c r="F261" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>1</v>
+      </c>
+      <c r="B262">
+        <v>2018</v>
+      </c>
+      <c r="C262">
+        <v>1</v>
+      </c>
+      <c r="D262" t="s">
+        <v>8</v>
+      </c>
+      <c r="E262" t="s">
+        <v>40</v>
+      </c>
+      <c r="F262" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>1</v>
+      </c>
+      <c r="B263">
+        <v>2018</v>
+      </c>
+      <c r="C263">
+        <v>1</v>
+      </c>
+      <c r="D263" t="s">
+        <v>8</v>
+      </c>
+      <c r="E263" t="s">
+        <v>40</v>
+      </c>
+      <c r="F263" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>1</v>
+      </c>
+      <c r="B264">
+        <v>2018</v>
+      </c>
+      <c r="C264">
+        <v>1</v>
+      </c>
+      <c r="D264" t="s">
+        <v>15</v>
+      </c>
+      <c r="E264" t="s">
+        <v>40</v>
+      </c>
+      <c r="F264" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>1</v>
+      </c>
+      <c r="B265">
+        <v>2018</v>
+      </c>
+      <c r="C265">
+        <v>1</v>
+      </c>
+      <c r="D265" t="s">
+        <v>15</v>
+      </c>
+      <c r="E265" t="s">
+        <v>40</v>
+      </c>
+      <c r="F265" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>1</v>
+      </c>
+      <c r="B266">
+        <v>2018</v>
+      </c>
+      <c r="C266">
+        <v>1</v>
+      </c>
+      <c r="D266" t="s">
+        <v>15</v>
+      </c>
+      <c r="E266" t="s">
+        <v>40</v>
+      </c>
+      <c r="F266" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>1</v>
+      </c>
+      <c r="B267">
+        <v>2018</v>
+      </c>
+      <c r="C267">
+        <v>1</v>
+      </c>
+      <c r="D267" t="s">
+        <v>15</v>
+      </c>
+      <c r="E267" t="s">
+        <v>40</v>
+      </c>
+      <c r="F267" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>1</v>
+      </c>
+      <c r="B268">
+        <v>2018</v>
+      </c>
+      <c r="C268">
+        <v>1</v>
+      </c>
+      <c r="D268" t="s">
+        <v>15</v>
+      </c>
+      <c r="E268" t="s">
+        <v>40</v>
+      </c>
+      <c r="F268" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>1</v>
+      </c>
+      <c r="B269">
+        <v>2018</v>
+      </c>
+      <c r="C269">
+        <v>1</v>
+      </c>
+      <c r="D269" t="s">
+        <v>15</v>
+      </c>
+      <c r="E269" t="s">
+        <v>40</v>
+      </c>
+      <c r="F269" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>1</v>
+      </c>
+      <c r="B270">
+        <v>2018</v>
+      </c>
+      <c r="C270">
+        <v>1</v>
+      </c>
+      <c r="D270" t="s">
+        <v>15</v>
+      </c>
+      <c r="E270" t="s">
+        <v>40</v>
+      </c>
+      <c r="F270" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>1</v>
+      </c>
+      <c r="B271">
+        <v>2018</v>
+      </c>
+      <c r="C271">
+        <v>1</v>
+      </c>
+      <c r="D271" t="s">
+        <v>15</v>
+      </c>
+      <c r="E271" t="s">
+        <v>40</v>
+      </c>
+      <c r="F271" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>1</v>
+      </c>
+      <c r="B272">
+        <v>2018</v>
+      </c>
+      <c r="C272">
+        <v>1</v>
+      </c>
+      <c r="D272" t="s">
+        <v>15</v>
+      </c>
+      <c r="E272" t="s">
+        <v>40</v>
+      </c>
+      <c r="F272" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -6458,6 +6816,7 @@
     <hyperlink ref="F156" r:id="rId128" xr:uid="{48323B38-D479-46AC-B219-915FBB77DFD8}"/>
     <hyperlink ref="F157" r:id="rId129" xr:uid="{C6A97135-FE75-4E74-9E08-30F3469A9E3C}"/>
     <hyperlink ref="F158" r:id="rId130" xr:uid="{CC0C1FB7-F9E6-4F27-A344-9D3DC76C05F7}"/>
+    <hyperlink ref="F242" r:id="rId131" xr:uid="{51F30ED5-92FB-4DE2-9E07-BA91DC10FB48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
results of Feb 2018
</commit_message>
<xml_diff>
--- a/journal_URL.xlsx
+++ b/journal_URL.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117DA65A-2C0B-46DE-9F0C-C2EE4CAAFE4E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="376">
   <si>
     <t>journal</t>
   </si>
@@ -901,6 +902,252 @@
   </si>
   <si>
     <t>https://academic.oup.com/jas/article/96/1/364/4818649</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/animal/article/influence-of-paraaminohippuric-acid-analysis-on-net-portaldrained-viscera-flux-of-nutrients-in-pigs/391061E8F12B0180E6439F556DBF13B1</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/animal/article/mode-of-action-of-saccharomyces-cerevisiae-in-enteric-methane-mitigation-in-pigs/6B94DD8C201E573606049858C15807EA</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/animal/article/grape-pomace-improves-performance-antioxidant-status-fecal-microbiota-and-meat-quality-of-piglets/A33DCD65196A681881FAB71704AA5C2B</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/animal/article/growth-meat-and-feed-efficiency-traits-of-lambs-born-to-ewes-submitted-to-energy-restriction-during-midgestation/BF8E65D4490CA7AC3CD9F5338526F915</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/animal/article/impact-of-animal-density-on-cattle-nutrition-in-dry-mediterranean-rangelands-a-faecal-nearir-spectroscopyaided-study/84D25BE8B56B42EC8D236D4CF5639096</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/animal/article/postweaning-feed-efficiency-decreased-in-progeny-of-higher-milk-yielding-beef-cows/CCED17F555C5D61913188485866D3C51</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/animal/article/effect-of-dietary-addition-of-nitrate-or-increase-in-lipid-concentrations-alone-or-in-combination-on-performance-and-methane-emissions-of-beef-cattle/042AD9AB21B81F20CB3AD11450179DB5</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117302742</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308957</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117312555</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117304170</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308878</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117308489</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117315894</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117310106</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117311872</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S037784011731101X</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S037784011731026X</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117311756</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117306363</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117309379</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117311604</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117311318</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117311379</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0377840117310271</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23771</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23801</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23796</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23800</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23798</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23810</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23765</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23805</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23820</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23802</t>
+  </si>
+  <si>
+    <t>https://www.ajas.info/journal/view.php?number=23828</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/545/4828053</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/558/4828104</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/570/4828152</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/579/4827968</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/591/4833885</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/600/4827736</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/653/4829573</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/670/4829313</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/684/4828210</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/694/4828034</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/705/4828072</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/715/4828030</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/728/4834025</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/739/4827744</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/751/4828173</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jas/article/96/2/752/4827738</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217310664</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217311487</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217311037</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217311116</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217311189</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217311050</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217310950</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217311256</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217311621</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217310986</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217310998</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217311323</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217310767</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S002203021731158X</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217310858</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022030217311499</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S187114131730361X</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1871141317303815</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1871141317303621</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1871141317303657</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1871141317303700</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/2/522/4683670</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/2/531/4609701</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/2/540/4601755</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/2/549/4601756</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/2/557/4565737</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/2/568/4675275</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/2/578/4739531</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/2/592/4739537</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ps/article/97/2/599/4739538</t>
   </si>
 </sst>
 </file>
@@ -1230,11 +1477,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F272"/>
+  <dimension ref="A1:F355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D279" sqref="D279"/>
+      <pane ySplit="1" topLeftCell="A326" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D350" sqref="D350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6682,6 +6929,1666 @@
       </c>
       <c r="F272" t="s">
         <v>293</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>57</v>
+      </c>
+      <c r="B273">
+        <v>2018</v>
+      </c>
+      <c r="C273">
+        <v>2</v>
+      </c>
+      <c r="D273" t="s">
+        <v>8</v>
+      </c>
+      <c r="E273" t="s">
+        <v>40</v>
+      </c>
+      <c r="F273" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>57</v>
+      </c>
+      <c r="B274">
+        <v>2018</v>
+      </c>
+      <c r="C274">
+        <v>2</v>
+      </c>
+      <c r="D274" t="s">
+        <v>8</v>
+      </c>
+      <c r="E274" t="s">
+        <v>40</v>
+      </c>
+      <c r="F274" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>57</v>
+      </c>
+      <c r="B275">
+        <v>2018</v>
+      </c>
+      <c r="C275">
+        <v>2</v>
+      </c>
+      <c r="D275" t="s">
+        <v>8</v>
+      </c>
+      <c r="E275" t="s">
+        <v>40</v>
+      </c>
+      <c r="F275" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>57</v>
+      </c>
+      <c r="B276">
+        <v>2018</v>
+      </c>
+      <c r="C276">
+        <v>2</v>
+      </c>
+      <c r="D276" t="s">
+        <v>15</v>
+      </c>
+      <c r="E276" t="s">
+        <v>40</v>
+      </c>
+      <c r="F276" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>57</v>
+      </c>
+      <c r="B277">
+        <v>2018</v>
+      </c>
+      <c r="C277">
+        <v>2</v>
+      </c>
+      <c r="D277" t="s">
+        <v>15</v>
+      </c>
+      <c r="E277" t="s">
+        <v>40</v>
+      </c>
+      <c r="F277" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>57</v>
+      </c>
+      <c r="B278">
+        <v>2018</v>
+      </c>
+      <c r="C278">
+        <v>2</v>
+      </c>
+      <c r="D278" t="s">
+        <v>15</v>
+      </c>
+      <c r="E278" t="s">
+        <v>40</v>
+      </c>
+      <c r="F278" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>57</v>
+      </c>
+      <c r="B279">
+        <v>2018</v>
+      </c>
+      <c r="C279">
+        <v>2</v>
+      </c>
+      <c r="D279" t="s">
+        <v>15</v>
+      </c>
+      <c r="E279" t="s">
+        <v>40</v>
+      </c>
+      <c r="F279" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>90</v>
+      </c>
+      <c r="B280">
+        <v>2018</v>
+      </c>
+      <c r="C280">
+        <v>2</v>
+      </c>
+      <c r="D280" t="s">
+        <v>15</v>
+      </c>
+      <c r="E280" t="s">
+        <v>40</v>
+      </c>
+      <c r="F280" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>90</v>
+      </c>
+      <c r="B281">
+        <v>2018</v>
+      </c>
+      <c r="C281">
+        <v>2</v>
+      </c>
+      <c r="D281" t="s">
+        <v>15</v>
+      </c>
+      <c r="E281" t="s">
+        <v>40</v>
+      </c>
+      <c r="F281" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>90</v>
+      </c>
+      <c r="B282">
+        <v>2018</v>
+      </c>
+      <c r="C282">
+        <v>2</v>
+      </c>
+      <c r="D282" t="s">
+        <v>15</v>
+      </c>
+      <c r="E282" t="s">
+        <v>40</v>
+      </c>
+      <c r="F282" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>90</v>
+      </c>
+      <c r="B283">
+        <v>2018</v>
+      </c>
+      <c r="C283">
+        <v>2</v>
+      </c>
+      <c r="D283" t="s">
+        <v>15</v>
+      </c>
+      <c r="E283" t="s">
+        <v>40</v>
+      </c>
+      <c r="F283" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>90</v>
+      </c>
+      <c r="B284">
+        <v>2018</v>
+      </c>
+      <c r="C284">
+        <v>2</v>
+      </c>
+      <c r="D284" t="s">
+        <v>15</v>
+      </c>
+      <c r="E284" t="s">
+        <v>21</v>
+      </c>
+      <c r="F284" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>90</v>
+      </c>
+      <c r="B285">
+        <v>2018</v>
+      </c>
+      <c r="C285">
+        <v>2</v>
+      </c>
+      <c r="D285" t="s">
+        <v>15</v>
+      </c>
+      <c r="E285" t="s">
+        <v>40</v>
+      </c>
+      <c r="F285" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>90</v>
+      </c>
+      <c r="B286">
+        <v>2018</v>
+      </c>
+      <c r="C286">
+        <v>2</v>
+      </c>
+      <c r="D286" t="s">
+        <v>15</v>
+      </c>
+      <c r="E286" t="s">
+        <v>40</v>
+      </c>
+      <c r="F286" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>90</v>
+      </c>
+      <c r="B287">
+        <v>2018</v>
+      </c>
+      <c r="C287">
+        <v>2</v>
+      </c>
+      <c r="D287" t="s">
+        <v>15</v>
+      </c>
+      <c r="E287" t="s">
+        <v>40</v>
+      </c>
+      <c r="F287" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>90</v>
+      </c>
+      <c r="B288">
+        <v>2018</v>
+      </c>
+      <c r="C288">
+        <v>2</v>
+      </c>
+      <c r="D288" t="s">
+        <v>8</v>
+      </c>
+      <c r="E288" t="s">
+        <v>40</v>
+      </c>
+      <c r="F288" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>90</v>
+      </c>
+      <c r="B289">
+        <v>2018</v>
+      </c>
+      <c r="C289">
+        <v>2</v>
+      </c>
+      <c r="D289" t="s">
+        <v>8</v>
+      </c>
+      <c r="E289" t="s">
+        <v>40</v>
+      </c>
+      <c r="F289" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>90</v>
+      </c>
+      <c r="B290">
+        <v>2018</v>
+      </c>
+      <c r="C290">
+        <v>2</v>
+      </c>
+      <c r="D290" t="s">
+        <v>8</v>
+      </c>
+      <c r="E290" t="s">
+        <v>40</v>
+      </c>
+      <c r="F290" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>90</v>
+      </c>
+      <c r="B291">
+        <v>2018</v>
+      </c>
+      <c r="C291">
+        <v>2</v>
+      </c>
+      <c r="D291" t="s">
+        <v>8</v>
+      </c>
+      <c r="E291" t="s">
+        <v>40</v>
+      </c>
+      <c r="F291" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>90</v>
+      </c>
+      <c r="B292">
+        <v>2018</v>
+      </c>
+      <c r="C292">
+        <v>2</v>
+      </c>
+      <c r="D292" t="s">
+        <v>8</v>
+      </c>
+      <c r="E292" t="s">
+        <v>40</v>
+      </c>
+      <c r="F292" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>90</v>
+      </c>
+      <c r="B293">
+        <v>2018</v>
+      </c>
+      <c r="C293">
+        <v>2</v>
+      </c>
+      <c r="D293" t="s">
+        <v>8</v>
+      </c>
+      <c r="E293" t="s">
+        <v>40</v>
+      </c>
+      <c r="F293" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>90</v>
+      </c>
+      <c r="B294">
+        <v>2018</v>
+      </c>
+      <c r="C294">
+        <v>2</v>
+      </c>
+      <c r="D294" t="s">
+        <v>8</v>
+      </c>
+      <c r="E294" t="s">
+        <v>40</v>
+      </c>
+      <c r="F294" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>90</v>
+      </c>
+      <c r="B295">
+        <v>2018</v>
+      </c>
+      <c r="C295">
+        <v>2</v>
+      </c>
+      <c r="D295" t="s">
+        <v>8</v>
+      </c>
+      <c r="E295" t="s">
+        <v>40</v>
+      </c>
+      <c r="F295" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>90</v>
+      </c>
+      <c r="B296">
+        <v>2018</v>
+      </c>
+      <c r="C296">
+        <v>2</v>
+      </c>
+      <c r="D296" t="s">
+        <v>8</v>
+      </c>
+      <c r="E296" t="s">
+        <v>40</v>
+      </c>
+      <c r="F296" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>90</v>
+      </c>
+      <c r="B297">
+        <v>2018</v>
+      </c>
+      <c r="C297">
+        <v>2</v>
+      </c>
+      <c r="D297" t="s">
+        <v>8</v>
+      </c>
+      <c r="E297" t="s">
+        <v>40</v>
+      </c>
+      <c r="F297" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>90</v>
+      </c>
+      <c r="B298">
+        <v>2018</v>
+      </c>
+      <c r="C298">
+        <v>2</v>
+      </c>
+      <c r="D298" t="s">
+        <v>15</v>
+      </c>
+      <c r="E298" t="s">
+        <v>40</v>
+      </c>
+      <c r="F298" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>41</v>
+      </c>
+      <c r="B299">
+        <v>2018</v>
+      </c>
+      <c r="C299">
+        <v>2</v>
+      </c>
+      <c r="D299" t="s">
+        <v>15</v>
+      </c>
+      <c r="E299" t="s">
+        <v>40</v>
+      </c>
+      <c r="F299" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>41</v>
+      </c>
+      <c r="B300">
+        <v>2018</v>
+      </c>
+      <c r="C300">
+        <v>2</v>
+      </c>
+      <c r="D300" t="s">
+        <v>15</v>
+      </c>
+      <c r="E300" t="s">
+        <v>40</v>
+      </c>
+      <c r="F300" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>41</v>
+      </c>
+      <c r="B301">
+        <v>2018</v>
+      </c>
+      <c r="C301">
+        <v>2</v>
+      </c>
+      <c r="D301" t="s">
+        <v>15</v>
+      </c>
+      <c r="E301" t="s">
+        <v>40</v>
+      </c>
+      <c r="F301" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>41</v>
+      </c>
+      <c r="B302">
+        <v>2018</v>
+      </c>
+      <c r="C302">
+        <v>2</v>
+      </c>
+      <c r="D302" t="s">
+        <v>15</v>
+      </c>
+      <c r="E302" t="s">
+        <v>40</v>
+      </c>
+      <c r="F302" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>41</v>
+      </c>
+      <c r="B303">
+        <v>2018</v>
+      </c>
+      <c r="C303">
+        <v>2</v>
+      </c>
+      <c r="D303" t="s">
+        <v>15</v>
+      </c>
+      <c r="E303" t="s">
+        <v>40</v>
+      </c>
+      <c r="F303" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>41</v>
+      </c>
+      <c r="B304">
+        <v>2018</v>
+      </c>
+      <c r="C304">
+        <v>2</v>
+      </c>
+      <c r="D304" t="s">
+        <v>8</v>
+      </c>
+      <c r="E304" t="s">
+        <v>40</v>
+      </c>
+      <c r="F304" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>41</v>
+      </c>
+      <c r="B305">
+        <v>2018</v>
+      </c>
+      <c r="C305">
+        <v>2</v>
+      </c>
+      <c r="D305" t="s">
+        <v>8</v>
+      </c>
+      <c r="E305" t="s">
+        <v>40</v>
+      </c>
+      <c r="F305" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>41</v>
+      </c>
+      <c r="B306">
+        <v>2018</v>
+      </c>
+      <c r="C306">
+        <v>2</v>
+      </c>
+      <c r="D306" t="s">
+        <v>8</v>
+      </c>
+      <c r="E306" t="s">
+        <v>40</v>
+      </c>
+      <c r="F306" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>41</v>
+      </c>
+      <c r="B307">
+        <v>2018</v>
+      </c>
+      <c r="C307">
+        <v>2</v>
+      </c>
+      <c r="D307" t="s">
+        <v>8</v>
+      </c>
+      <c r="E307" t="s">
+        <v>40</v>
+      </c>
+      <c r="F307" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>41</v>
+      </c>
+      <c r="B308">
+        <v>2018</v>
+      </c>
+      <c r="C308">
+        <v>2</v>
+      </c>
+      <c r="D308" t="s">
+        <v>8</v>
+      </c>
+      <c r="E308" t="s">
+        <v>40</v>
+      </c>
+      <c r="F308" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>41</v>
+      </c>
+      <c r="B309">
+        <v>2018</v>
+      </c>
+      <c r="C309">
+        <v>2</v>
+      </c>
+      <c r="D309" t="s">
+        <v>8</v>
+      </c>
+      <c r="E309" t="s">
+        <v>40</v>
+      </c>
+      <c r="F309" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>1</v>
+      </c>
+      <c r="B310">
+        <v>2018</v>
+      </c>
+      <c r="C310">
+        <v>2</v>
+      </c>
+      <c r="D310" t="s">
+        <v>8</v>
+      </c>
+      <c r="E310" t="s">
+        <v>40</v>
+      </c>
+      <c r="F310" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>1</v>
+      </c>
+      <c r="B311">
+        <v>2018</v>
+      </c>
+      <c r="C311">
+        <v>2</v>
+      </c>
+      <c r="D311" t="s">
+        <v>8</v>
+      </c>
+      <c r="E311" t="s">
+        <v>40</v>
+      </c>
+      <c r="F311" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>1</v>
+      </c>
+      <c r="B312">
+        <v>2018</v>
+      </c>
+      <c r="C312">
+        <v>2</v>
+      </c>
+      <c r="D312" t="s">
+        <v>8</v>
+      </c>
+      <c r="E312" t="s">
+        <v>40</v>
+      </c>
+      <c r="F312" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>1</v>
+      </c>
+      <c r="B313">
+        <v>2018</v>
+      </c>
+      <c r="C313">
+        <v>2</v>
+      </c>
+      <c r="D313" t="s">
+        <v>8</v>
+      </c>
+      <c r="E313" t="s">
+        <v>40</v>
+      </c>
+      <c r="F313" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>1</v>
+      </c>
+      <c r="B314">
+        <v>2018</v>
+      </c>
+      <c r="C314">
+        <v>2</v>
+      </c>
+      <c r="D314" t="s">
+        <v>8</v>
+      </c>
+      <c r="E314" t="s">
+        <v>40</v>
+      </c>
+      <c r="F314" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>1</v>
+      </c>
+      <c r="B315">
+        <v>2018</v>
+      </c>
+      <c r="C315">
+        <v>2</v>
+      </c>
+      <c r="D315" t="s">
+        <v>8</v>
+      </c>
+      <c r="E315" t="s">
+        <v>40</v>
+      </c>
+      <c r="F315" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>1</v>
+      </c>
+      <c r="B316">
+        <v>2018</v>
+      </c>
+      <c r="C316">
+        <v>2</v>
+      </c>
+      <c r="D316" t="s">
+        <v>15</v>
+      </c>
+      <c r="E316" t="s">
+        <v>40</v>
+      </c>
+      <c r="F316" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>1</v>
+      </c>
+      <c r="B317">
+        <v>2018</v>
+      </c>
+      <c r="C317">
+        <v>2</v>
+      </c>
+      <c r="D317" t="s">
+        <v>15</v>
+      </c>
+      <c r="E317" t="s">
+        <v>40</v>
+      </c>
+      <c r="F317" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>1</v>
+      </c>
+      <c r="B318">
+        <v>2018</v>
+      </c>
+      <c r="C318">
+        <v>2</v>
+      </c>
+      <c r="D318" t="s">
+        <v>15</v>
+      </c>
+      <c r="E318" t="s">
+        <v>40</v>
+      </c>
+      <c r="F318" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>1</v>
+      </c>
+      <c r="B319">
+        <v>2018</v>
+      </c>
+      <c r="C319">
+        <v>2</v>
+      </c>
+      <c r="D319" t="s">
+        <v>15</v>
+      </c>
+      <c r="E319" t="s">
+        <v>40</v>
+      </c>
+      <c r="F319" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>1</v>
+      </c>
+      <c r="B320">
+        <v>2018</v>
+      </c>
+      <c r="C320">
+        <v>2</v>
+      </c>
+      <c r="D320" t="s">
+        <v>15</v>
+      </c>
+      <c r="E320" t="s">
+        <v>40</v>
+      </c>
+      <c r="F320" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>1</v>
+      </c>
+      <c r="B321">
+        <v>2018</v>
+      </c>
+      <c r="C321">
+        <v>2</v>
+      </c>
+      <c r="D321" t="s">
+        <v>15</v>
+      </c>
+      <c r="E321" t="s">
+        <v>40</v>
+      </c>
+      <c r="F321" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>1</v>
+      </c>
+      <c r="B322">
+        <v>2018</v>
+      </c>
+      <c r="C322">
+        <v>2</v>
+      </c>
+      <c r="D322" t="s">
+        <v>8</v>
+      </c>
+      <c r="E322" t="s">
+        <v>21</v>
+      </c>
+      <c r="F322" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>1</v>
+      </c>
+      <c r="B323">
+        <v>2018</v>
+      </c>
+      <c r="C323">
+        <v>2</v>
+      </c>
+      <c r="D323" t="s">
+        <v>15</v>
+      </c>
+      <c r="E323" t="s">
+        <v>21</v>
+      </c>
+      <c r="F323" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>1</v>
+      </c>
+      <c r="B324">
+        <v>2018</v>
+      </c>
+      <c r="C324">
+        <v>2</v>
+      </c>
+      <c r="D324" t="s">
+        <v>15</v>
+      </c>
+      <c r="E324" t="s">
+        <v>21</v>
+      </c>
+      <c r="F324" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>1</v>
+      </c>
+      <c r="B325">
+        <v>2018</v>
+      </c>
+      <c r="C325">
+        <v>2</v>
+      </c>
+      <c r="D325" t="s">
+        <v>15</v>
+      </c>
+      <c r="E325" t="s">
+        <v>21</v>
+      </c>
+      <c r="F325" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>38</v>
+      </c>
+      <c r="B326">
+        <v>2018</v>
+      </c>
+      <c r="C326">
+        <v>2</v>
+      </c>
+      <c r="D326" t="s">
+        <v>15</v>
+      </c>
+      <c r="E326" t="s">
+        <v>21</v>
+      </c>
+      <c r="F326" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>38</v>
+      </c>
+      <c r="B327">
+        <v>2018</v>
+      </c>
+      <c r="C327">
+        <v>2</v>
+      </c>
+      <c r="D327" t="s">
+        <v>15</v>
+      </c>
+      <c r="E327" t="s">
+        <v>40</v>
+      </c>
+      <c r="F327" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>38</v>
+      </c>
+      <c r="B328">
+        <v>2018</v>
+      </c>
+      <c r="C328">
+        <v>2</v>
+      </c>
+      <c r="D328" t="s">
+        <v>15</v>
+      </c>
+      <c r="E328" t="s">
+        <v>40</v>
+      </c>
+      <c r="F328" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>38</v>
+      </c>
+      <c r="B329">
+        <v>2018</v>
+      </c>
+      <c r="C329">
+        <v>2</v>
+      </c>
+      <c r="D329" t="s">
+        <v>15</v>
+      </c>
+      <c r="E329" t="s">
+        <v>40</v>
+      </c>
+      <c r="F329" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>38</v>
+      </c>
+      <c r="B330">
+        <v>2018</v>
+      </c>
+      <c r="C330">
+        <v>2</v>
+      </c>
+      <c r="D330" t="s">
+        <v>15</v>
+      </c>
+      <c r="E330" t="s">
+        <v>40</v>
+      </c>
+      <c r="F330" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>38</v>
+      </c>
+      <c r="B331">
+        <v>2018</v>
+      </c>
+      <c r="C331">
+        <v>2</v>
+      </c>
+      <c r="D331" t="s">
+        <v>15</v>
+      </c>
+      <c r="E331" t="s">
+        <v>40</v>
+      </c>
+      <c r="F331" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>38</v>
+      </c>
+      <c r="B332">
+        <v>2018</v>
+      </c>
+      <c r="C332">
+        <v>2</v>
+      </c>
+      <c r="D332" t="s">
+        <v>15</v>
+      </c>
+      <c r="E332" t="s">
+        <v>40</v>
+      </c>
+      <c r="F332" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>38</v>
+      </c>
+      <c r="B333">
+        <v>2018</v>
+      </c>
+      <c r="C333">
+        <v>2</v>
+      </c>
+      <c r="D333" t="s">
+        <v>15</v>
+      </c>
+      <c r="E333" t="s">
+        <v>40</v>
+      </c>
+      <c r="F333" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>38</v>
+      </c>
+      <c r="B334">
+        <v>2018</v>
+      </c>
+      <c r="C334">
+        <v>2</v>
+      </c>
+      <c r="D334" t="s">
+        <v>15</v>
+      </c>
+      <c r="E334" t="s">
+        <v>40</v>
+      </c>
+      <c r="F334" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>38</v>
+      </c>
+      <c r="B335">
+        <v>2018</v>
+      </c>
+      <c r="C335">
+        <v>2</v>
+      </c>
+      <c r="D335" t="s">
+        <v>15</v>
+      </c>
+      <c r="E335" t="s">
+        <v>40</v>
+      </c>
+      <c r="F335" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>38</v>
+      </c>
+      <c r="B336">
+        <v>2018</v>
+      </c>
+      <c r="C336">
+        <v>2</v>
+      </c>
+      <c r="D336" t="s">
+        <v>15</v>
+      </c>
+      <c r="E336" t="s">
+        <v>40</v>
+      </c>
+      <c r="F336" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>38</v>
+      </c>
+      <c r="B337">
+        <v>2018</v>
+      </c>
+      <c r="C337">
+        <v>2</v>
+      </c>
+      <c r="D337" t="s">
+        <v>15</v>
+      </c>
+      <c r="E337" t="s">
+        <v>40</v>
+      </c>
+      <c r="F337" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>38</v>
+      </c>
+      <c r="B338">
+        <v>2018</v>
+      </c>
+      <c r="C338">
+        <v>2</v>
+      </c>
+      <c r="D338" t="s">
+        <v>15</v>
+      </c>
+      <c r="E338" t="s">
+        <v>40</v>
+      </c>
+      <c r="F338" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>38</v>
+      </c>
+      <c r="B339">
+        <v>2018</v>
+      </c>
+      <c r="C339">
+        <v>2</v>
+      </c>
+      <c r="D339" t="s">
+        <v>15</v>
+      </c>
+      <c r="E339" t="s">
+        <v>40</v>
+      </c>
+      <c r="F339" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>38</v>
+      </c>
+      <c r="B340">
+        <v>2018</v>
+      </c>
+      <c r="C340">
+        <v>2</v>
+      </c>
+      <c r="D340" t="s">
+        <v>15</v>
+      </c>
+      <c r="E340" t="s">
+        <v>40</v>
+      </c>
+      <c r="F340" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>38</v>
+      </c>
+      <c r="B341">
+        <v>2018</v>
+      </c>
+      <c r="C341">
+        <v>2</v>
+      </c>
+      <c r="D341" t="s">
+        <v>15</v>
+      </c>
+      <c r="E341" t="s">
+        <v>40</v>
+      </c>
+      <c r="F341" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>91</v>
+      </c>
+      <c r="B342">
+        <v>2018</v>
+      </c>
+      <c r="C342">
+        <v>2</v>
+      </c>
+      <c r="D342" t="s">
+        <v>15</v>
+      </c>
+      <c r="E342" t="s">
+        <v>40</v>
+      </c>
+      <c r="F342" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>91</v>
+      </c>
+      <c r="B343">
+        <v>2018</v>
+      </c>
+      <c r="C343">
+        <v>2</v>
+      </c>
+      <c r="D343" t="s">
+        <v>8</v>
+      </c>
+      <c r="E343" t="s">
+        <v>21</v>
+      </c>
+      <c r="F343" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>91</v>
+      </c>
+      <c r="B344">
+        <v>2018</v>
+      </c>
+      <c r="C344">
+        <v>2</v>
+      </c>
+      <c r="D344" t="s">
+        <v>8</v>
+      </c>
+      <c r="E344" t="s">
+        <v>40</v>
+      </c>
+      <c r="F344" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>91</v>
+      </c>
+      <c r="B345">
+        <v>2018</v>
+      </c>
+      <c r="C345">
+        <v>2</v>
+      </c>
+      <c r="D345" t="s">
+        <v>8</v>
+      </c>
+      <c r="E345" t="s">
+        <v>40</v>
+      </c>
+      <c r="F345" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>91</v>
+      </c>
+      <c r="B346">
+        <v>2018</v>
+      </c>
+      <c r="C346">
+        <v>2</v>
+      </c>
+      <c r="D346" t="s">
+        <v>8</v>
+      </c>
+      <c r="E346" t="s">
+        <v>40</v>
+      </c>
+      <c r="F346" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>66</v>
+      </c>
+      <c r="B347">
+        <v>2018</v>
+      </c>
+      <c r="C347">
+        <v>2</v>
+      </c>
+      <c r="D347" t="s">
+        <v>8</v>
+      </c>
+      <c r="E347" t="s">
+        <v>40</v>
+      </c>
+      <c r="F347" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>66</v>
+      </c>
+      <c r="B348">
+        <v>2018</v>
+      </c>
+      <c r="C348">
+        <v>2</v>
+      </c>
+      <c r="D348" t="s">
+        <v>8</v>
+      </c>
+      <c r="E348" t="s">
+        <v>40</v>
+      </c>
+      <c r="F348" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>66</v>
+      </c>
+      <c r="B349">
+        <v>2018</v>
+      </c>
+      <c r="C349">
+        <v>2</v>
+      </c>
+      <c r="D349" t="s">
+        <v>8</v>
+      </c>
+      <c r="E349" t="s">
+        <v>40</v>
+      </c>
+      <c r="F349" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>66</v>
+      </c>
+      <c r="B350">
+        <v>2018</v>
+      </c>
+      <c r="C350">
+        <v>2</v>
+      </c>
+      <c r="D350" t="s">
+        <v>8</v>
+      </c>
+      <c r="E350" t="s">
+        <v>40</v>
+      </c>
+      <c r="F350" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>66</v>
+      </c>
+      <c r="B351">
+        <v>2018</v>
+      </c>
+      <c r="C351">
+        <v>2</v>
+      </c>
+      <c r="D351" t="s">
+        <v>8</v>
+      </c>
+      <c r="E351" t="s">
+        <v>40</v>
+      </c>
+      <c r="F351" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>66</v>
+      </c>
+      <c r="B352">
+        <v>2018</v>
+      </c>
+      <c r="C352">
+        <v>2</v>
+      </c>
+      <c r="D352" t="s">
+        <v>8</v>
+      </c>
+      <c r="E352" t="s">
+        <v>40</v>
+      </c>
+      <c r="F352" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>66</v>
+      </c>
+      <c r="B353">
+        <v>2018</v>
+      </c>
+      <c r="C353">
+        <v>2</v>
+      </c>
+      <c r="D353" t="s">
+        <v>8</v>
+      </c>
+      <c r="E353" t="s">
+        <v>40</v>
+      </c>
+      <c r="F353" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>66</v>
+      </c>
+      <c r="B354">
+        <v>2018</v>
+      </c>
+      <c r="C354">
+        <v>2</v>
+      </c>
+      <c r="D354" t="s">
+        <v>8</v>
+      </c>
+      <c r="E354" t="s">
+        <v>40</v>
+      </c>
+      <c r="F354" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>66</v>
+      </c>
+      <c r="B355">
+        <v>2018</v>
+      </c>
+      <c r="C355">
+        <v>2</v>
+      </c>
+      <c r="D355" t="s">
+        <v>8</v>
+      </c>
+      <c r="E355" t="s">
+        <v>40</v>
+      </c>
+      <c r="F355" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>